<commit_message>
Test accuracy when training model using half and a quarter of the LOs
</commit_message>
<xml_diff>
--- a/outputs/all_lo_mappings.xlsx
+++ b/outputs/all_lo_mappings.xlsx
@@ -486,7 +486,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>[('justify', 'Valuing'), ('work', 'Valuing'), ('collaborate', 'Organisation'), ('demonstrate', 'Valuing'), ('report', 'Valuing')]</t>
+          <t>[('justify', 'Organisation'), ('work', 'Valuing'), ('collaborate', 'Organisation'), ('demonstrate', 'Responding'), ('report', 'Responding')]</t>
         </is>
       </c>
     </row>
@@ -506,17 +506,17 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Applying</t>
+          <t>Analysing</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>[('produce', 'Creating'), ('apply', 'Applying')]</t>
+          <t>[('produce', 'Creating'), ('apply', 'Analysing')]</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>[('create', 'Creating'), ('summarise', 'Understanding'), ('derive', 'Applying'), ('query', 'Analysing'), ('order', 'Remembering')]</t>
+          <t>[('create', 'Creating'), ('summarise', 'Applying'), ('derive', 'Analysing'), ('query', 'Analysing'), ('order', 'Applying')]</t>
         </is>
       </c>
     </row>
@@ -536,17 +536,17 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Applying</t>
+          <t>Analysing</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>[('engage', 'Verb not mapped'), ('demonstrate', 'Applying'), ('act', 'Applying')]</t>
+          <t>[('engage', 'Creating'), ('demonstrate', 'Analysing'), ('act', 'Analysing')]</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>[('monitor', 'Evaluating'), ('file', 'Analysing'), ('prepare', 'Applying'), ('point', 'Remembering'), ('generate', 'Creating')]</t>
+          <t>[('monitor', 'Evaluating'), ('file', 'Analysing'), ('prepare', 'Analysing'), ('point', 'Remembering'), ('generate', 'Creating')]</t>
         </is>
       </c>
     </row>
@@ -566,17 +566,17 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Applying</t>
+          <t>Analysing</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>[('demonstrate', 'Applying'), ('drive', 'Verb not mapped'), ('include', 'Verb not mapped'), ('limit', 'Verb not mapped'), ('serve', 'Verb not mapped')]</t>
+          <t>[('demonstrate', 'Analysing'), ('drive', 'Verb not mapped'), ('include', 'Verb not mapped'), ('limit', 'Verb not mapped'), ('serve', 'Verb not mapped')]</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>[('lecture', 'Evaluating'), ('value', 'Evaluating'), ('prepare', 'Applying'), ('discuss', 'Understanding'), ('generate', 'Creating')]</t>
+          <t>[('lecture', 'Evaluating'), ('value', 'Evaluating'), ('prepare', 'Analysing'), ('discuss', 'Applying'), ('satisfy', 'Evaluating')]</t>
         </is>
       </c>
     </row>
@@ -591,22 +591,22 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Affective</t>
+          <t>Cognitive</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Organisation</t>
+          <t>Analysing</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>[('understand', 'Verb not mapped'), ('test', 'Organisation'), ('relate', 'Organisation')]</t>
+          <t>[('understand', 'Verb not mapped'), ('test', 'Analysing'), ('relate', 'Applying')]</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>[('establish', 'Organisation'), ('allow', 'Responding'), ('perform', 'Characterisation'), ('support', 'Valuing'), ('study', 'Valuing')]</t>
+          <t>[('provide', 'Applying'), ('establish', 'Analysing'), ('perform', 'Creating'), ('support', 'Evaluating'), ('produce', 'Creating')]</t>
         </is>
       </c>
     </row>
@@ -636,7 +636,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>[('collaborate', 'Organisation'), ('monitor', 'Valuing'), ('act', 'Characterisation'), ('generate', 'Organisation'), ('respond', 'Responding')]</t>
+          <t>[('collaborate', 'Organisation'), ('satisfy', 'Organisation'), ('monitor', 'Valuing'), ('engage', 'Characterisation'), ('define', 'Responding')]</t>
         </is>
       </c>
     </row>
@@ -666,7 +666,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>[('characterise', 'Understanding'), ('transfer', 'Applying'), ('rate', 'Evaluating'), ('document', 'Analysing'), ('evaluate', 'Evaluating')]</t>
+          <t>[('characterise', 'Applying'), ('transfer', 'Analysing'), ('discern', 'Analysing'), ('rate', 'Evaluating'), ('document', 'Analysing')]</t>
         </is>
       </c>
     </row>
@@ -681,22 +681,22 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Affective</t>
+          <t>Cognitive</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Organisation</t>
+          <t>Creating</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>[('consider', 'Organisation'), ('create', 'Verb not mapped'), ('challenge', 'Characterisation'), ('integrate', 'Organisation'), ('accommodate', 'Verb not mapped'), ('differ', 'Verb not mapped')]</t>
+          <t>[('consider', 'Evaluating'), ('create', 'Creating'), ('challenge', 'Verb not mapped'), ('integrate', 'Evaluating'), ('accommodate', 'Verb not mapped'), ('differ', 'Verb not mapped')]</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>[('guide', 'Valuing'), ('establish', 'Organisation'), ('discuss', 'Responding'), ('perform', 'Characterisation'), ('monitor', 'Valuing')]</t>
+          <t>[('establish', 'Analysing'), ('produce', 'Creating'), ('lecture', 'Evaluating'), ('discuss', 'Applying'), ('interface', 'Evaluating')]</t>
         </is>
       </c>
     </row>
@@ -716,17 +716,17 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Applying</t>
+          <t>Analysing</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>[('demonstrate', 'Applying'), ('align', 'Verb not mapped'), ('deliver', 'Verb not mapped')]</t>
+          <t>[('demonstrate', 'Analysing'), ('align', 'Verb not mapped'), ('deliver', 'Verb not mapped')]</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>[('value', 'Evaluating'), ('point', 'Remembering'), ('produce', 'Creating'), ('improve', 'Evaluating'), ('act', 'Applying')]</t>
+          <t>[('value', 'Evaluating'), ('discern', 'Analysing'), ('point', 'Remembering'), ('produce', 'Creating'), ('improve', 'Evaluating')]</t>
         </is>
       </c>
     </row>
@@ -746,12 +746,12 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Applying</t>
+          <t>Analysing</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>[('understand', 'Verb not mapped'), ('apply', 'Applying'), ('enable', 'Verb not mapped')]</t>
+          <t>[('understand', 'Verb not mapped'), ('apply', 'Analysing'), ('enable', 'Verb not mapped')]</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -786,7 +786,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>[('adopt', 'Valuing'), ('collaborate', 'Organisation'), ('perform', 'Characterisation'), ('act', 'Characterisation'), ('respond', 'Responding')]</t>
+          <t>[('contrast', 'Organisation'), ('mitigate', 'Characterisation'), ('adopt', 'Valuing'), ('collaborate', 'Organisation'), ('perform', 'Characterisation')]</t>
         </is>
       </c>
     </row>
@@ -806,17 +806,17 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Remembering</t>
+          <t>Applying</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>[('relate', 'Remembering')]</t>
+          <t>[('relate', 'Applying')]</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>[('provide', 'Applying'), ('establish', 'Applying'), ('perform', 'Creating'), ('support', 'Evaluating'), ('produce', 'Creating')]</t>
+          <t>[('provide', 'Applying'), ('establish', 'Analysing'), ('perform', 'Creating'), ('support', 'Evaluating'), ('produce', 'Creating')]</t>
         </is>
       </c>
     </row>
@@ -836,17 +836,17 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Applying</t>
+          <t>Analysing</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>[('solve', 'Applying'), ('relate', 'Remembering')]</t>
+          <t>[('solve', 'Analysing'), ('relate', 'Applying')]</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>[('provide', 'Applying'), ('establish', 'Applying'), ('perform', 'Creating'), ('support', 'Evaluating'), ('produce', 'Creating')]</t>
+          <t>[('provide', 'Applying'), ('establish', 'Analysing'), ('perform', 'Creating'), ('support', 'Evaluating'), ('produce', 'Creating')]</t>
         </is>
       </c>
     </row>
@@ -866,17 +866,17 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Applying</t>
+          <t>Analysing</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>[('apply', 'Applying')]</t>
+          <t>[('apply', 'Analysing')]</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>[('create', 'Creating'), ('summarise', 'Understanding'), ('derive', 'Applying'), ('query', 'Analysing'), ('order', 'Remembering')]</t>
+          <t>[('create', 'Creating'), ('summarise', 'Applying'), ('derive', 'Analysing'), ('query', 'Analysing'), ('order', 'Applying')]</t>
         </is>
       </c>
     </row>
@@ -896,17 +896,17 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Applying</t>
+          <t>Analysing</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>[('operate', 'Applying'), ('evaluate', 'Evaluating')]</t>
+          <t>[('operate', 'Analysing'), ('evaluate', 'Evaluating')]</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>[('experiment', 'Analysing'), ('compare', 'Understanding'), ('file', 'Analysing'), ('respond', 'Understanding'), ('document', 'Analysing')]</t>
+          <t>[('experiment', 'Analysing'), ('compare', 'Applying'), ('file', 'Analysing'), ('respond', 'Understanding'), ('document', 'Analysing')]</t>
         </is>
       </c>
     </row>
@@ -922,22 +922,22 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>SOLO</t>
+          <t>Cognitive</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Relational</t>
+          <t>Evaluating</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>[('address', 'Relational')]</t>
+          <t>[('address', 'Evaluating')]</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>[('mitigate', 'Extended Abstract'), ('perform', 'Relational'), ('choose', 'Unistructural'), ('characterise', 'Relational'), ('generate', 'Extended Abstract')]</t>
+          <t>[('adopt', 'Evaluating'), ('monitor', 'Evaluating'), ('experiment', 'Analysing'), ('group', 'Analysing'), ('devise', 'Evaluating')]</t>
         </is>
       </c>
     </row>
@@ -957,17 +957,17 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Understanding</t>
+          <t>Applying</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>[('describe', 'Understanding')]</t>
+          <t>[('describe', 'Applying')]</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>[('lecture', 'Evaluating'), ('interface', 'Evaluating'), ('simulate', 'Applying'), ('produce', 'Creating'), ('trace', 'Remembering')]</t>
+          <t>[('lecture', 'Evaluating'), ('interface', 'Evaluating'), ('simulate', 'Analysing'), ('produce', 'Creating'), ('trace', 'Remembering')]</t>
         </is>
       </c>
     </row>
@@ -988,17 +988,17 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Applying</t>
+          <t>Analysing</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>[('apply', 'Applying'), ('learn', 'Verb not mapped'), ('design', 'Creating')]</t>
+          <t>[('apply', 'Analysing'), ('learn', 'Verb not mapped'), ('design', 'Creating')]</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>[('summarise', 'Understanding'), ('order', 'Remembering'), ('propose', 'Creating'), ('apply', 'Applying'), ('compute', 'Applying')]</t>
+          <t>[('summarise', 'Applying'), ('order', 'Applying'), ('propose', 'Evaluating'), ('apply', 'Analysing'), ('compute', 'Analysing')]</t>
         </is>
       </c>
     </row>
@@ -1028,7 +1028,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>[('factor', 'Understanding'), ('integrate', 'Evaluating'), ('review', 'Remembering'), ('plan', 'Creating'), ('devise', 'Evaluating')]</t>
+          <t>[('factor', 'Understanding'), ('integrate', 'Evaluating'), ('review', 'Analysing'), ('plan', 'Creating'), ('devise', 'Evaluating')]</t>
         </is>
       </c>
     </row>
@@ -1058,7 +1058,7 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>[('explore', 'Analysing'), ('choose', 'Applying'), ('experiment', 'Analysing'), ('change', 'Applying'), ('extract', 'Analysing')]</t>
+          <t>[('explore', 'Analysing'), ('choose', 'Applying'), ('experiment', 'Analysing'), ('change', 'Analysing'), ('extract', 'Analysing')]</t>
         </is>
       </c>
     </row>
@@ -1088,7 +1088,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>[('justify', 'Valuing'), ('work', 'Valuing'), ('collaborate', 'Organisation'), ('demonstrate', 'Valuing'), ('report', 'Valuing')]</t>
+          <t>[('justify', 'Organisation'), ('work', 'Valuing'), ('collaborate', 'Organisation'), ('demonstrate', 'Responding'), ('report', 'Responding')]</t>
         </is>
       </c>
     </row>
@@ -1118,7 +1118,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>[('explore', 'Analysing'), ('choose', 'Applying'), ('experiment', 'Analysing'), ('change', 'Applying'), ('extract', 'Analysing')]</t>
+          <t>[('explore', 'Analysing'), ('choose', 'Applying'), ('experiment', 'Analysing'), ('change', 'Analysing'), ('extract', 'Analysing')]</t>
         </is>
       </c>
     </row>
@@ -1133,22 +1133,22 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Affective</t>
+          <t>Cognitive</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Organisation</t>
+          <t>Evaluating</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>[('generate', 'Organisation'), ('meet', 'Receiving')]</t>
+          <t>[('generate', 'Creating'), ('meet', 'Remembering')]</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>[('query', 'Valuing'), ('agree', 'Responding'), ('follow', 'Receiving'), ('meet', 'Receiving'), ('generate', 'Organisation')]</t>
+          <t>[('query', 'Analysing'), ('ensure', 'Analysing'), ('back', 'Applying'), ('produce', 'Creating'), ('generate', 'Creating')]</t>
         </is>
       </c>
     </row>
@@ -1178,7 +1178,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>[('summarise', 'Understanding'), ('order', 'Remembering'), ('propose', 'Creating'), ('apply', 'Applying'), ('compute', 'Applying')]</t>
+          <t>[('summarise', 'Applying'), ('order', 'Applying'), ('propose', 'Evaluating'), ('apply', 'Analysing'), ('compute', 'Analysing')]</t>
         </is>
       </c>
     </row>
@@ -1198,17 +1198,17 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Creating</t>
+          <t>Evaluating</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>[('construct', 'Creating')]</t>
+          <t>[('construct', 'Evaluating')]</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>[('debug', 'Evaluating'), ('interface', 'Evaluating'), ('summarise', 'Understanding'), ('simulate', 'Applying'), ('improve', 'Evaluating')]</t>
+          <t>[('debug', 'Evaluating'), ('interface', 'Evaluating'), ('reduce', 'Evaluating'), ('summarise', 'Applying'), ('simulate', 'Analysing')]</t>
         </is>
       </c>
     </row>
@@ -1223,22 +1223,22 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Affective</t>
+          <t>Cognitive</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Organisation</t>
+          <t>Evaluating</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>[('generate', 'Organisation')]</t>
+          <t>[('generate', 'Creating')]</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>[('prepare', 'Organisation'), ('monitor', 'Valuing'), ('agree', 'Responding'), ('adopt', 'Valuing'), ('relay', 'Responding')]</t>
+          <t>[('prepare', 'Analysing'), ('monitor', 'Evaluating'), ('lecture', 'Evaluating'), ('adopt', 'Evaluating'), ('operate', 'Analysing')]</t>
         </is>
       </c>
     </row>
@@ -1268,7 +1268,7 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>[('discuss', 'Responding'), ('relay', 'Responding'), ('characterise', 'Characterisation'), ('agree', 'Responding'), ('monitor', 'Valuing')]</t>
+          <t>[('value', 'Characterisation'), ('mitigate', 'Characterisation'), ('define', 'Responding'), ('satisfy', 'Organisation'), ('discuss', 'Responding')]</t>
         </is>
       </c>
     </row>
@@ -1283,22 +1283,22 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Cognitive</t>
+          <t>Affective</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Applying</t>
+          <t>Valuing</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>[('identify', 'Understanding'), ('calculate', 'Applying'), ('subject', 'Verb not mapped'), ('accord', 'Verb not mapped')]</t>
+          <t>[('identify', 'Receiving'), ('calculate', 'Valuing'), ('subject', 'Verb not mapped'), ('accord', 'Verb not mapped')]</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>[('factor', 'Understanding'), ('back', 'Applying'), ('adopt', 'Evaluating'), ('discuss', 'Understanding'), ('assign', 'Applying')]</t>
+          <t>[('guide', 'Valuing'), ('adopt', 'Valuing'), ('discuss', 'Responding'), ('agree', 'Responding'), ('prepare', 'Responding')]</t>
         </is>
       </c>
     </row>
@@ -1328,7 +1328,7 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>[('extract', 'Analysing'), ('interface', 'Evaluating'), ('file', 'Analysing'), ('example', 'Understanding'), ('trace', 'Remembering')]</t>
+          <t>[('reduce', 'Evaluating'), ('extract', 'Analysing'), ('interface', 'Evaluating'), ('file', 'Analysing'), ('example', 'Understanding')]</t>
         </is>
       </c>
     </row>
@@ -1358,7 +1358,7 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>[('experiment', 'Analysing'), ('derive', 'Applying'), ('improve', 'Evaluating'), ('lecture', 'Evaluating'), ('establish', 'Applying')]</t>
+          <t>[('experiment', 'Analysing'), ('derive', 'Analysing'), ('improve', 'Evaluating'), ('lecture', 'Evaluating'), ('establish', 'Analysing')]</t>
         </is>
       </c>
     </row>
@@ -1378,17 +1378,17 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Understanding</t>
+          <t>Applying</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>[('describe', 'Understanding'), ('include', 'Verb not mapped')]</t>
+          <t>[('describe', 'Applying'), ('include', 'Verb not mapped')]</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>[('factor', 'Understanding'), ('integrate', 'Evaluating'), ('review', 'Remembering'), ('plan', 'Creating'), ('devise', 'Evaluating')]</t>
+          <t>[('factor', 'Understanding'), ('integrate', 'Evaluating'), ('review', 'Analysing'), ('plan', 'Creating'), ('devise', 'Evaluating')]</t>
         </is>
       </c>
     </row>
@@ -1408,17 +1408,17 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Understanding</t>
+          <t>Applying</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>[('discuss', 'Understanding'), ('include', 'Verb not mapped')]</t>
+          <t>[('discuss', 'Applying'), ('include', 'Verb not mapped')]</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>[('factor', 'Understanding'), ('integrate', 'Evaluating'), ('review', 'Remembering'), ('plan', 'Creating'), ('devise', 'Evaluating')]</t>
+          <t>[('factor', 'Understanding'), ('integrate', 'Evaluating'), ('review', 'Analysing'), ('plan', 'Creating'), ('devise', 'Evaluating')]</t>
         </is>
       </c>
     </row>
@@ -1448,7 +1448,7 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>[('relay', 'Responding'), ('characterise', 'Characterisation'), ('describe', 'Receiving'), ('identify', 'Receiving'), ('verify', 'Characterisation')]</t>
+          <t>[('discern', 'Valuing'), ('relay', 'Responding'), ('reduce', 'Organisation'), ('characterise', 'Valuing'), ('describe', 'Receiving')]</t>
         </is>
       </c>
     </row>
@@ -1468,17 +1468,17 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Applying</t>
+          <t>Analysing</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>[('apply', 'Applying'), ('include', 'Verb not mapped')]</t>
+          <t>[('apply', 'Analysing'), ('include', 'Verb not mapped')]</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>[('factor', 'Understanding'), ('integrate', 'Evaluating'), ('review', 'Remembering'), ('plan', 'Creating'), ('devise', 'Evaluating')]</t>
+          <t>[('factor', 'Understanding'), ('integrate', 'Evaluating'), ('review', 'Analysing'), ('plan', 'Creating'), ('devise', 'Evaluating')]</t>
         </is>
       </c>
     </row>
@@ -1533,7 +1533,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>[('evaluate', 'Valuing'), ('apply', 'Verb not mapped'), ('plan', 'Organisation'), ('organise', 'Organisation'), ('manage', 'Organisation')]</t>
+          <t>[('evaluate', 'Organisation'), ('apply', 'Valuing'), ('plan', 'Organisation'), ('organise', 'Organisation'), ('manage', 'Organisation')]</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -1588,12 +1588,12 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Understanding</t>
+          <t>Applying</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>[('discuss', 'Understanding')]</t>
+          <t>[('discuss', 'Applying')]</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -1624,12 +1624,12 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>[('construct', 'Creating'), ('deploy', 'Verb not mapped'), ('link', 'Verb not mapped')]</t>
+          <t>[('construct', 'Evaluating'), ('deploy', 'Verb not mapped'), ('link', 'Verb not mapped')]</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>[('list', 'Remembering'), ('file', 'Analysing'), ('extract', 'Analysing'), ('utilise', 'Applying'), ('monitor', 'Evaluating')]</t>
+          <t>[('list', 'Applying'), ('file', 'Analysing'), ('extract', 'Analysing'), ('utilise', 'Applying'), ('monitor', 'Evaluating')]</t>
         </is>
       </c>
     </row>
@@ -1645,22 +1645,22 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>SOLO</t>
+          <t>Cognitive</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Relational</t>
+          <t>Evaluating</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>[('construct', 'Relational'), ('target', 'Verb not mapped')]</t>
+          <t>[('construct', 'Evaluating'), ('target', 'Verb not mapped')]</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>[('reduce', 'Relational'), ('sequence', 'Multistructural'), ('mitigate', 'Extended Abstract'), ('calculate', 'Relational'), ('simulate', 'Extended Abstract')]</t>
+          <t>[('reduce', 'Evaluating'), ('file', 'Analysing'), ('interface', 'Evaluating'), ('sequence', 'Applying'), ('extract', 'Analysing')]</t>
         </is>
       </c>
     </row>
@@ -1691,7 +1691,7 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>[('extract', 'Analysing'), ('interface', 'Evaluating'), ('file', 'Analysing'), ('example', 'Understanding'), ('trace', 'Remembering')]</t>
+          <t>[('reduce', 'Evaluating'), ('extract', 'Analysing'), ('interface', 'Evaluating'), ('file', 'Analysing'), ('example', 'Understanding')]</t>
         </is>
       </c>
     </row>
@@ -1707,22 +1707,22 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>SOLO</t>
+          <t>Cognitive</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Multistructural</t>
+          <t>Applying</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>[('describe', 'Multistructural'), ('solve', 'Multistructural')]</t>
+          <t>[('describe', 'Applying'), ('solve', 'Analysing')]</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>[('discern', 'Multistructural'), ('appreciate', 'Relational'), ('translate', 'Relational'), ('mitigate', 'Extended Abstract'), ('generate', 'Extended Abstract')]</t>
+          <t>[('interface', 'Evaluating'), ('trace', 'Remembering'), ('complete', 'Applying'), ('document', 'Analysing'), ('utilise', 'Applying')]</t>
         </is>
       </c>
     </row>
@@ -1742,17 +1742,17 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Applying</t>
+          <t>Analysing</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>[('solve', 'Applying'), ('design', 'Creating'), ('use', 'Applying')]</t>
+          <t>[('solve', 'Analysing'), ('design', 'Creating'), ('use', 'Applying')]</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>[('extract', 'Analysing'), ('interface', 'Evaluating'), ('file', 'Analysing'), ('example', 'Understanding'), ('trace', 'Remembering')]</t>
+          <t>[('reduce', 'Evaluating'), ('extract', 'Analysing'), ('interface', 'Evaluating'), ('file', 'Analysing'), ('example', 'Understanding')]</t>
         </is>
       </c>
     </row>
@@ -1768,22 +1768,22 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>SOLO</t>
+          <t>Cognitive</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Relational</t>
+          <t>Analysing</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>[('analyse', 'Relational'), ('partition', 'Relational'), ('interpret', 'Relational'), ('solve', 'Multistructural'), ('apply', 'Relational'), ('create', 'Extended Abstract')]</t>
+          <t>[('analyse', 'Analysing'), ('partition', 'Evaluating'), ('interpret', 'Analysing'), ('solve', 'Analysing'), ('apply', 'Analysing'), ('create', 'Creating')]</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>[('order', 'Unistructural'), ('value', 'Extended Abstract'), ('observe', 'Relational'), ('generate', 'Extended Abstract'), ('validate', 'Extended Abstract')]</t>
+          <t>[('order', 'Applying'), ('value', 'Evaluating'), ('lecture', 'Evaluating'), ('improve', 'Evaluating'), ('observe', 'Applying')]</t>
         </is>
       </c>
     </row>
@@ -1799,22 +1799,22 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>SOLO</t>
+          <t>Affective</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Relational</t>
+          <t>Organisation</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>[('construct', 'Relational'), ('compute', 'Relational'), ('reflect', 'Extended Abstract'), ('conclude', 'Relational')]</t>
+          <t>[('construct', 'Organisation'), ('compute', 'Valuing'), ('reflect', 'Characterisation'), ('conclude', 'Organisation')]</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>[('compute', 'Relational'), ('select', 'Multistructural'), ('synthesise', 'Extended Abstract'), ('generate', 'Extended Abstract'), ('order', 'Unistructural')]</t>
+          <t>[('compute', 'Valuing'), ('select', 'Responding'), ('prepare', 'Responding'), ('relay', 'Responding'), ('synthesise', 'Organisation')]</t>
         </is>
       </c>
     </row>
@@ -1845,7 +1845,7 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>[('conclude', 'Creating'), ('research', 'Analysing'), ('interpret', 'Applying'), ('summarise', 'Understanding'), ('group', 'Analysing')]</t>
+          <t>[('issue', 'Analysing'), ('conclude', 'Creating'), ('research', 'Analysing'), ('interpret', 'Analysing'), ('summarise', 'Applying')]</t>
         </is>
       </c>
     </row>
@@ -1866,17 +1866,17 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Understanding</t>
+          <t>Applying</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>[('describe', 'Understanding'), ('define', 'Remembering'), ('summarise', 'Understanding')]</t>
+          <t>[('describe', 'Applying'), ('define', 'Applying'), ('summarise', 'Applying')]</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>[('derive', 'Applying'), ('order', 'Remembering'), ('improve', 'Evaluating'), ('change', 'Applying'), ('lecture', 'Evaluating')]</t>
+          <t>[('derive', 'Analysing'), ('order', 'Applying'), ('improve', 'Evaluating'), ('change', 'Analysing'), ('lecture', 'Evaluating')]</t>
         </is>
       </c>
     </row>
@@ -1896,17 +1896,17 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Applying</t>
+          <t>Analysing</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>[('determine', 'Analysing'), ('compute', 'Applying'), ('make', 'Creating')]</t>
+          <t>[('determine', 'Analysing'), ('compute', 'Analysing'), ('make', 'Creating')]</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>[('order', 'Remembering'), ('compute', 'Applying'), ('make', 'Creating'), ('select', 'Evaluating'), ('conclude', 'Creating')]</t>
+          <t>[('order', 'Applying'), ('compute', 'Analysing'), ('make', 'Creating'), ('select', 'Applying'), ('conclude', 'Creating')]</t>
         </is>
       </c>
     </row>
@@ -1927,17 +1927,17 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Applying</t>
+          <t>Analysing</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>[('interpret', 'Applying'), ('apply', 'Applying'), ('supervise', 'Verb not mapped')]</t>
+          <t>[('interpret', 'Analysing'), ('apply', 'Analysing'), ('supervise', 'Verb not mapped')]</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>[('create', 'Creating'), ('summarise', 'Understanding'), ('derive', 'Applying'), ('query', 'Analysing'), ('order', 'Remembering')]</t>
+          <t>[('create', 'Creating'), ('summarise', 'Applying'), ('derive', 'Analysing'), ('query', 'Analysing'), ('order', 'Applying')]</t>
         </is>
       </c>
     </row>
@@ -1953,22 +1953,22 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>SOLO</t>
+          <t>Cognitive</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Extended Abstract</t>
+          <t>Analysing</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>[('simulate', 'Extended Abstract'), ('use', 'Relational'), ('design', 'Extended Abstract'), ('base', 'Verb not mapped'), ('extract', 'Verb not mapped')]</t>
+          <t>[('simulate', 'Analysing'), ('use', 'Applying'), ('design', 'Creating'), ('base', 'Verb not mapped'), ('extract', 'Analysing')]</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>[('mitigate', 'Extended Abstract'), ('calculate', 'Relational'), ('sequence', 'Multistructural'), ('translate', 'Relational'), ('perform', 'Relational')]</t>
+          <t>[('trace', 'Remembering'), ('interface', 'Evaluating'), ('example', 'Understanding'), ('mitigate', 'Creating'), ('file', 'Analysing')]</t>
         </is>
       </c>
     </row>
@@ -1988,17 +1988,17 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Analysing</t>
+          <t>Applying</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>[('differentiate', 'Analysing'), ('reflect', 'Evaluating')]</t>
+          <t>[('differentiate', 'Applying'), ('reflect', 'Evaluating')]</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>[('prepare', 'Applying'), ('generate', 'Creating'), ('sequence', 'Applying'), ('trace', 'Remembering'), ('specify', 'Evaluating')]</t>
+          <t>[('prepare', 'Analysing'), ('generate', 'Creating'), ('sequence', 'Applying'), ('trace', 'Remembering'), ('specify', 'Evaluating')]</t>
         </is>
       </c>
     </row>
@@ -2013,22 +2013,22 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Affective</t>
+          <t>Cognitive</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Organisation</t>
+          <t>Analysing</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>[('generate', 'Organisation'), ('document', 'Verb not mapped')]</t>
+          <t>[('generate', 'Creating'), ('document', 'Analysing')]</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>[('adopt', 'Valuing'), ('monitor', 'Valuing'), ('respond', 'Responding'), ('generate', 'Organisation'), ('prepare', 'Organisation')]</t>
+          <t>[('adopt', 'Evaluating'), ('monitor', 'Evaluating'), ('respond', 'Understanding'), ('interface', 'Evaluating'), ('generate', 'Creating')]</t>
         </is>
       </c>
     </row>
@@ -2043,22 +2043,22 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>SOLO</t>
+          <t>Psychomotor</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Extended Abstract</t>
+          <t>Origination</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>[('design', 'Extended Abstract'), ('appraise', 'Extended Abstract')]</t>
+          <t>[('design', 'Origination'), ('appraise', 'Origination')]</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>[('choose', 'Unistructural'), ('assess', 'Extended Abstract'), ('verify', 'Relational'), ('calculate', 'Relational'), ('sequence', 'Multistructural')]</t>
+          <t>[('choose', 'Perception'), ('change', 'Mechanism'), ('assess', 'Origination'), ('verify', 'Adaptation'), ('calculate', 'Mechanism')]</t>
         </is>
       </c>
     </row>
@@ -2074,22 +2074,22 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Cognitive</t>
+          <t>Affective</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Applying</t>
+          <t>Responding</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>[('demonstrate', 'Applying'), ('use', 'Applying')]</t>
+          <t>[('demonstrate', 'Responding'), ('use', 'Responding')]</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>[('extract', 'Analysing'), ('interface', 'Evaluating'), ('file', 'Analysing'), ('example', 'Understanding'), ('trace', 'Remembering')]</t>
+          <t>[('reduce', 'Organisation'), ('construct', 'Organisation'), ('translate', 'Responding'), ('discern', 'Valuing'), ('explain', 'Responding')]</t>
         </is>
       </c>
     </row>
@@ -2120,7 +2120,7 @@
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>[('rate', 'Evaluating'), ('trace', 'Remembering'), ('factor', 'Understanding'), ('discuss', 'Understanding'), ('sequence', 'Applying')]</t>
+          <t>[('rate', 'Evaluating'), ('trace', 'Remembering'), ('factor', 'Understanding'), ('discuss', 'Applying'), ('sequence', 'Applying')]</t>
         </is>
       </c>
     </row>
@@ -2141,17 +2141,17 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Understanding</t>
+          <t>Applying</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>[('describe', 'Understanding'), ('exploit', 'Verb not mapped')]</t>
+          <t>[('describe', 'Applying'), ('exploit', 'Verb not mapped')]</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>[('rate', 'Evaluating'), ('trace', 'Remembering'), ('factor', 'Understanding'), ('discuss', 'Understanding'), ('sequence', 'Applying')]</t>
+          <t>[('rate', 'Evaluating'), ('trace', 'Remembering'), ('factor', 'Understanding'), ('discuss', 'Applying'), ('sequence', 'Applying')]</t>
         </is>
       </c>
     </row>
@@ -2167,22 +2167,22 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Cognitive</t>
+          <t>SOLO</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Understanding</t>
+          <t>Unistructural</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>[('explain', 'Understanding'), ('characterise', 'Understanding'), ('describe', 'Understanding'), ('include', 'Verb not mapped'), ('allow', 'Verb not mapped'), ('identify', 'Understanding')]</t>
+          <t>[('explain', 'Unistructural'), ('characterise', 'Unistructural'), ('describe', 'Unistructural'), ('include', 'Verb not mapped'), ('allow', 'Verb not mapped'), ('identify', 'Unistructural')]</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>[('factor', 'Understanding'), ('assess', 'Evaluating'), ('review', 'Remembering'), ('group', 'Analysing'), ('define', 'Remembering')]</t>
+          <t>[('assess', 'Extended Abstract'), ('address', 'Relational'), ('review', 'Multistructural'), ('define', 'Unistructural'), ('characterise', 'Unistructural')]</t>
         </is>
       </c>
     </row>
@@ -2197,22 +2197,22 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>SOLO</t>
+          <t>Affective</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Relational</t>
+          <t>Valuing</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>[('compute', 'Relational'), ('support', 'Verb not mapped'), ('relate', 'Relational')]</t>
+          <t>[('compute', 'Valuing'), ('support', 'Valuing'), ('relate', 'Responding')]</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>[('perform', 'Relational'), ('relate', 'Relational'), ('validate', 'Extended Abstract'), ('differentiate', 'Relational'), ('derive', 'Relational')]</t>
+          <t>[('establish', 'Valuing'), ('allow', 'Responding'), ('perform', 'Characterisation'), ('support', 'Valuing'), ('relate', 'Responding')]</t>
         </is>
       </c>
     </row>
@@ -2233,12 +2233,12 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Understanding</t>
+          <t>Applying</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>[('explain', 'Understanding'), ('include', 'Verb not mapped'), ('enable', 'Verb not mapped')]</t>
+          <t>[('explain', 'Applying'), ('include', 'Verb not mapped'), ('enable', 'Verb not mapped')]</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -2274,7 +2274,7 @@
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>[('lecture', 'Evaluating'), ('trace', 'Remembering'), ('specify', 'Evaluating'), ('consider', 'Evaluating'), ('derive', 'Applying')]</t>
+          <t>[('lecture', 'Evaluating'), ('trace', 'Remembering'), ('specify', 'Evaluating'), ('consider', 'Evaluating'), ('derive', 'Analysing')]</t>
         </is>
       </c>
     </row>
@@ -2295,17 +2295,17 @@
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Understanding</t>
+          <t>Applying</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>[('describe', 'Understanding')]</t>
+          <t>[('describe', 'Applying')]</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>[('lecture', 'Evaluating'), ('interface', 'Evaluating'), ('simulate', 'Applying'), ('produce', 'Creating'), ('trace', 'Remembering')]</t>
+          <t>[('lecture', 'Evaluating'), ('interface', 'Evaluating'), ('simulate', 'Analysing'), ('produce', 'Creating'), ('trace', 'Remembering')]</t>
         </is>
       </c>
     </row>
@@ -2320,22 +2320,22 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>SOLO</t>
+          <t>Cognitive</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Multistructural</t>
+          <t>Analysing</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>[('discern', 'Multistructural'), ('appreciate', 'Relational')]</t>
+          <t>[('discern', 'Analysing'), ('appreciate', 'Evaluating')]</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>[('discern', 'Multistructural'), ('appreciate', 'Relational'), ('sequence', 'Multistructural'), ('compare', 'Relational'), ('generate', 'Extended Abstract')]</t>
+          <t>[('rate', 'Evaluating'), ('discern', 'Analysing'), ('appreciate', 'Evaluating'), ('act', 'Analysing'), ('trace', 'Remembering')]</t>
         </is>
       </c>
     </row>
@@ -2356,17 +2356,17 @@
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Applying</t>
+          <t>Analysing</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>[('interpret', 'Applying'), ('apply', 'Applying')]</t>
+          <t>[('interpret', 'Analysing'), ('apply', 'Analysing')]</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>[('create', 'Creating'), ('summarise', 'Understanding'), ('derive', 'Applying'), ('query', 'Analysing'), ('order', 'Remembering')]</t>
+          <t>[('create', 'Creating'), ('summarise', 'Applying'), ('derive', 'Analysing'), ('query', 'Analysing'), ('order', 'Applying')]</t>
         </is>
       </c>
     </row>
@@ -2397,7 +2397,7 @@
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>[('summarise', 'Understanding'), ('order', 'Remembering'), ('propose', 'Creating'), ('apply', 'Applying'), ('compute', 'Applying')]</t>
+          <t>[('summarise', 'Applying'), ('order', 'Applying'), ('propose', 'Evaluating'), ('apply', 'Analysing'), ('compute', 'Analysing')]</t>
         </is>
       </c>
     </row>
@@ -2413,22 +2413,22 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Cognitive</t>
+          <t>Affective</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Applying</t>
+          <t>Responding</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>[('demonstrate', 'Applying'), ('use', 'Applying')]</t>
+          <t>[('demonstrate', 'Responding'), ('use', 'Responding')]</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>[('extract', 'Analysing'), ('interface', 'Evaluating'), ('file', 'Analysing'), ('example', 'Understanding'), ('trace', 'Remembering')]</t>
+          <t>[('reduce', 'Organisation'), ('construct', 'Organisation'), ('translate', 'Responding'), ('discern', 'Valuing'), ('explain', 'Responding')]</t>
         </is>
       </c>
     </row>
@@ -2459,7 +2459,7 @@
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>[('adopt', 'Evaluating'), ('devise', 'Evaluating'), ('lecture', 'Evaluating'), ('improve', 'Evaluating'), ('change', 'Applying')]</t>
+          <t>[('adopt', 'Evaluating'), ('devise', 'Evaluating'), ('lecture', 'Evaluating'), ('improve', 'Evaluating'), ('change', 'Analysing')]</t>
         </is>
       </c>
     </row>
@@ -2475,22 +2475,22 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>SOLO</t>
+          <t>Cognitive</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Relational</t>
+          <t>Applying</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>[('interpret', 'Relational'), ('summarise', 'Relational'), ('relate', 'Relational'), ('base', 'Verb not mapped')]</t>
+          <t>[('interpret', 'Analysing'), ('summarise', 'Applying'), ('relate', 'Applying'), ('base', 'Verb not mapped')]</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>[('perform', 'Relational'), ('validate', 'Extended Abstract'), ('differentiate', 'Relational'), ('transfer', 'Relational'), ('test', 'Unistructural')]</t>
+          <t>[('provide', 'Applying'), ('establish', 'Analysing'), ('perform', 'Creating'), ('support', 'Evaluating'), ('produce', 'Creating')]</t>
         </is>
       </c>
     </row>
@@ -2521,7 +2521,7 @@
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>[('lecture', 'Evaluating'), ('trace', 'Remembering'), ('specify', 'Evaluating'), ('consider', 'Evaluating'), ('derive', 'Applying')]</t>
+          <t>[('lecture', 'Evaluating'), ('trace', 'Remembering'), ('specify', 'Evaluating'), ('consider', 'Evaluating'), ('derive', 'Analysing')]</t>
         </is>
       </c>
     </row>
@@ -2537,22 +2537,22 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Cognitive</t>
+          <t>Affective</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Evaluating</t>
+          <t>Organisation</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>[('select', 'Evaluating'), ('develop', 'Creating'), ('base', 'Verb not mapped'), ('evaluate', 'Evaluating')]</t>
+          <t>[('select', 'Responding'), ('develop', 'Organisation'), ('base', 'Verb not mapped'), ('evaluate', 'Organisation')]</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>[('experiment', 'Analysing'), ('compare', 'Understanding'), ('file', 'Analysing'), ('respond', 'Understanding'), ('document', 'Analysing')]</t>
+          <t>[('compare', 'Responding'), ('respond', 'Responding'), ('prepare', 'Responding'), ('adopt', 'Valuing'), ('mitigate', 'Characterisation')]</t>
         </is>
       </c>
     </row>
@@ -2573,17 +2573,17 @@
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Creating</t>
+          <t>Applying</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>[('summarise', 'Understanding'), ('propose', 'Creating'), ('design', 'Creating')]</t>
+          <t>[('summarise', 'Applying'), ('propose', 'Evaluating'), ('design', 'Creating')]</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>[('summarise', 'Understanding'), ('order', 'Remembering'), ('design', 'Creating'), ('propose', 'Creating'), ('apply', 'Applying')]</t>
+          <t>[('summarise', 'Applying'), ('order', 'Applying'), ('design', 'Creating'), ('propose', 'Evaluating'), ('apply', 'Analysing')]</t>
         </is>
       </c>
     </row>
@@ -2603,17 +2603,17 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Applying</t>
+          <t>Analysing</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>[('apply', 'Applying'), ('design', 'Creating'), ('include', 'Verb not mapped')]</t>
+          <t>[('apply', 'Analysing'), ('design', 'Creating'), ('include', 'Verb not mapped')]</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>[('factor', 'Understanding'), ('integrate', 'Evaluating'), ('review', 'Remembering'), ('plan', 'Creating'), ('devise', 'Evaluating')]</t>
+          <t>[('factor', 'Understanding'), ('integrate', 'Evaluating'), ('review', 'Analysing'), ('plan', 'Creating'), ('devise', 'Evaluating')]</t>
         </is>
       </c>
     </row>
@@ -2644,7 +2644,7 @@
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>[('experiment', 'Analysing'), ('calculate', 'Applying'), ('file', 'Analysing'), ('change', 'Applying'), ('compare', 'Understanding')]</t>
+          <t>[('experiment', 'Analysing'), ('calculate', 'Analysing'), ('file', 'Analysing'), ('change', 'Analysing'), ('compare', 'Applying')]</t>
         </is>
       </c>
     </row>
@@ -2665,17 +2665,17 @@
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Applying</t>
+          <t>Analysing</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>[('design', 'Creating'), ('implement', 'Applying'), ('solve', 'Applying'), ('give', 'Understanding'), ('use', 'Applying')]</t>
+          <t>[('design', 'Creating'), ('implement', 'Analysing'), ('solve', 'Analysing'), ('give', 'Understanding'), ('use', 'Applying')]</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>[('extract', 'Analysing'), ('interface', 'Evaluating'), ('file', 'Analysing'), ('example', 'Understanding'), ('trace', 'Remembering')]</t>
+          <t>[('reduce', 'Evaluating'), ('extract', 'Analysing'), ('interface', 'Evaluating'), ('file', 'Analysing'), ('example', 'Understanding')]</t>
         </is>
       </c>
     </row>
@@ -2696,17 +2696,17 @@
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Applying</t>
+          <t>Analysing</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>[('conduct', 'Applying'), ('investigate', 'Analysing'), ('base', 'Verb not mapped')]</t>
+          <t>[('conduct', 'Analysing'), ('investigate', 'Analysing'), ('base', 'Verb not mapped')]</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>[('experiment', 'Analysing'), ('change', 'Applying'), ('improve', 'Evaluating'), ('assess', 'Evaluating'), ('collect', 'Applying')]</t>
+          <t>[('experiment', 'Analysing'), ('change', 'Analysing'), ('improve', 'Evaluating'), ('assess', 'Evaluating'), ('collect', 'Applying')]</t>
         </is>
       </c>
     </row>
@@ -2737,7 +2737,7 @@
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>[('experiment', 'Analysing'), ('compare', 'Understanding'), ('file', 'Analysing'), ('respond', 'Understanding'), ('document', 'Analysing')]</t>
+          <t>[('experiment', 'Analysing'), ('compare', 'Applying'), ('file', 'Analysing'), ('respond', 'Understanding'), ('document', 'Analysing')]</t>
         </is>
       </c>
     </row>
@@ -2757,17 +2757,17 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Understanding</t>
+          <t>Applying</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>[('describe', 'Understanding')]</t>
+          <t>[('describe', 'Applying')]</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>[('lecture', 'Evaluating'), ('interface', 'Evaluating'), ('simulate', 'Applying'), ('produce', 'Creating'), ('trace', 'Remembering')]</t>
+          <t>[('lecture', 'Evaluating'), ('interface', 'Evaluating'), ('simulate', 'Analysing'), ('produce', 'Creating'), ('trace', 'Remembering')]</t>
         </is>
       </c>
     </row>
@@ -2797,7 +2797,7 @@
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>[('contrast', 'Analysing'), ('define', 'Remembering'), ('interface', 'Evaluating'), ('compare', 'Understanding'), ('lecture', 'Evaluating')]</t>
+          <t>[('mitigate', 'Creating'), ('contrast', 'Analysing'), ('define', 'Applying'), ('interface', 'Evaluating'), ('compare', 'Applying')]</t>
         </is>
       </c>
     </row>
@@ -2827,7 +2827,7 @@
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>[('monitor', 'Evaluating'), ('trace', 'Remembering'), ('generate', 'Creating'), ('group', 'Analysing'), ('act', 'Applying')]</t>
+          <t>[('monitor', 'Evaluating'), ('trace', 'Remembering'), ('generate', 'Creating'), ('group', 'Analysing'), ('act', 'Analysing')]</t>
         </is>
       </c>
     </row>
@@ -2848,17 +2848,17 @@
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Applying</t>
+          <t>Analysing</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>[('apply', 'Applying')]</t>
+          <t>[('apply', 'Analysing')]</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>[('create', 'Creating'), ('summarise', 'Understanding'), ('derive', 'Applying'), ('query', 'Analysing'), ('order', 'Remembering')]</t>
+          <t>[('create', 'Creating'), ('summarise', 'Applying'), ('derive', 'Analysing'), ('query', 'Analysing'), ('order', 'Applying')]</t>
         </is>
       </c>
     </row>
@@ -2889,7 +2889,7 @@
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>[('experiment', 'Analysing'), ('calculate', 'Applying'), ('file', 'Analysing'), ('change', 'Applying'), ('compare', 'Understanding')]</t>
+          <t>[('experiment', 'Analysing'), ('calculate', 'Analysing'), ('file', 'Analysing'), ('change', 'Analysing'), ('compare', 'Applying')]</t>
         </is>
       </c>
     </row>
@@ -2909,17 +2909,17 @@
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>Organisation</t>
+          <t>Responding</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>[('prepare', 'Organisation'), ('present', 'Responding'), ('base', 'Verb not mapped'), ('derive', 'Verb not mapped')]</t>
+          <t>[('prepare', 'Responding'), ('present', 'Responding'), ('base', 'Verb not mapped'), ('derive', 'Valuing')]</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>[('study', 'Valuing'), ('order', 'Organisation'), ('relay', 'Responding'), ('adopt', 'Valuing'), ('prepare', 'Organisation')]</t>
+          <t>[('study', 'Responding'), ('sequence', 'Valuing'), ('order', 'Responding'), ('relay', 'Responding'), ('summarise', 'Responding')]</t>
         </is>
       </c>
     </row>
@@ -2939,17 +2939,17 @@
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Applying</t>
+          <t>Analysing</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>[('apply', 'Applying')]</t>
+          <t>[('apply', 'Analysing')]</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>[('create', 'Creating'), ('summarise', 'Understanding'), ('derive', 'Applying'), ('query', 'Analysing'), ('order', 'Remembering')]</t>
+          <t>[('create', 'Creating'), ('summarise', 'Applying'), ('derive', 'Analysing'), ('query', 'Analysing'), ('order', 'Applying')]</t>
         </is>
       </c>
     </row>
@@ -2964,22 +2964,22 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Cognitive</t>
+          <t>Psychomotor</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Understanding</t>
+          <t>Guided Response</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>[('demonstrate', 'Applying'), ('observe', 'Understanding')]</t>
+          <t>[('demonstrate', 'Guided Response'), ('observe', 'Guided Response')]</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>[('value', 'Evaluating'), ('discuss', 'Understanding'), ('improve', 'Evaluating'), ('act', 'Applying'), ('lecture', 'Evaluating')]</t>
+          <t>[('value', 'Origination'), ('satisfy', 'Adaptation'), ('discuss', 'Guided Response'), ('respond', 'Guided Response'), ('discern', 'Mechanism')]</t>
         </is>
       </c>
     </row>
@@ -2999,17 +2999,17 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Applying</t>
+          <t>Evaluating</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>[('value', 'Evaluating'), ('satisfy', 'Verb not mapped'), ('assign', 'Applying')]</t>
+          <t>[('value', 'Evaluating'), ('satisfy', 'Evaluating'), ('assign', 'Applying')]</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>[('assign', 'Applying'), ('back', 'Applying'), ('prepare', 'Applying'), ('act', 'Applying'), ('discuss', 'Understanding')]</t>
+          <t>[('satisfy', 'Evaluating'), ('assign', 'Applying'), ('back', 'Applying'), ('prepare', 'Analysing'), ('act', 'Analysing')]</t>
         </is>
       </c>
     </row>
@@ -3024,22 +3024,22 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Cognitive</t>
+          <t>Affective</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Applying</t>
+          <t>Responding</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>[('demonstrate', 'Applying'), ('communicate', 'Verb not mapped'), ('write', 'Applying')]</t>
+          <t>[('demonstrate', 'Responding'), ('communicate', 'Responding'), ('write', 'Responding')]</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>[('detail', 'Understanding'), ('generate', 'Creating'), ('prepare', 'Applying'), ('report', 'Understanding'), ('query', 'Analysing')]</t>
+          <t>[('generate', 'Organisation'), ('prepare', 'Responding'), ('report', 'Responding'), ('query', 'Valuing'), ('reduce', 'Organisation')]</t>
         </is>
       </c>
     </row>
@@ -3054,22 +3054,22 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Affective</t>
+          <t>Psychomotor</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Valuing</t>
+          <t>Guided Response</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>[('demonstrate', 'Valuing'), ('work', 'Valuing'), ('collaborate', 'Organisation')]</t>
+          <t>[('demonstrate', 'Guided Response'), ('work', 'Guided Response'), ('collaborate', 'Verb not mapped')]</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>[('guide', 'Valuing'), ('act', 'Characterisation'), ('respond', 'Responding'), ('monitor', 'Valuing'), ('generate', 'Organisation')]</t>
+          <t>[('respond', 'Guided Response'), ('generate', 'Origination'), ('define', 'Guided Response'), ('prepare', 'Guided Response'), ('trace', 'Guided Response')]</t>
         </is>
       </c>
     </row>
@@ -3084,22 +3084,22 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>SOLO</t>
+          <t>Cognitive</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Extended Abstract</t>
+          <t>Analysing</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>[('demonstrate', 'Extended Abstract'), ('engage', 'Extended Abstract')]</t>
+          <t>[('demonstrate', 'Analysing'), ('engage', 'Creating')]</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>[('generate', 'Extended Abstract'), ('value', 'Extended Abstract'), ('choose', 'Unistructural'), ('define', 'Multistructural'), ('satisfy', 'Relational')]</t>
+          <t>[('generate', 'Creating'), ('monitor', 'Evaluating'), ('ensure', 'Analysing'), ('produce', 'Creating'), ('detail', 'Understanding')]</t>
         </is>
       </c>
     </row>
@@ -3114,22 +3114,22 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Affective</t>
+          <t>SOLO</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>Receiving</t>
+          <t>Multistructural</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>[('identify', 'Receiving'), ('select', 'Receiving'), ('derive', 'Verb not mapped')]</t>
+          <t>[('identify', 'Unistructural'), ('select', 'Multistructural'), ('derive', 'Multistructural')]</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>[('study', 'Valuing'), ('order', 'Organisation'), ('relay', 'Responding'), ('adopt', 'Valuing'), ('prepare', 'Organisation')]</t>
+          <t>[('sequence', 'Multistructural'), ('order', 'Unistructural'), ('summarise', 'Unistructural'), ('mitigate', 'Extended Abstract'), ('compute', 'Multistructural')]</t>
         </is>
       </c>
     </row>
@@ -3149,17 +3149,17 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>Applying</t>
+          <t>Analysing</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>[('apply', 'Applying'), ('solve', 'Applying')]</t>
+          <t>[('apply', 'Analysing'), ('solve', 'Analysing')]</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>[('query', 'Analysing'), ('interface', 'Evaluating'), ('describe', 'Understanding'), ('group', 'Analysing'), ('generate', 'Creating')]</t>
+          <t>[('query', 'Analysing'), ('interface', 'Evaluating'), ('describe', 'Applying'), ('group', 'Analysing'), ('generate', 'Creating')]</t>
         </is>
       </c>
     </row>
@@ -3174,22 +3174,22 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Affective</t>
+          <t>Cognitive</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>Responding</t>
+          <t>Applying</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>[('discuss', 'Responding'), ('write', 'Responding')]</t>
+          <t>[('discuss', 'Applying'), ('write', 'Applying')]</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>[('generate', 'Organisation'), ('prepare', 'Organisation'), ('report', 'Valuing'), ('query', 'Valuing'), ('act', 'Characterisation')]</t>
+          <t>[('detail', 'Understanding'), ('generate', 'Creating'), ('conduct', 'Analysing'), ('prepare', 'Analysing'), ('report', 'Applying')]</t>
         </is>
       </c>
     </row>
@@ -3204,22 +3204,22 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>SOLO</t>
+          <t>Cognitive</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>Extended Abstract</t>
+          <t>Creating</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>[('engage', 'Extended Abstract')]</t>
+          <t>[('engage', 'Creating')]</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>[('generate', 'Extended Abstract'), ('value', 'Extended Abstract'), ('choose', 'Unistructural'), ('define', 'Multistructural'), ('satisfy', 'Relational')]</t>
+          <t>[('generate', 'Creating'), ('monitor', 'Evaluating'), ('ensure', 'Analysing'), ('produce', 'Creating'), ('detail', 'Understanding')]</t>
         </is>
       </c>
     </row>
@@ -3249,7 +3249,7 @@
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>[('conclude', 'Relational'), ('derive', 'Relational'), ('validate', 'Extended Abstract'), ('select', 'Multistructural'), ('order', 'Unistructural')]</t>
+          <t>[('conclude', 'Relational'), ('derive', 'Multistructural'), ('validate', 'Extended Abstract'), ('select', 'Multistructural'), ('order', 'Unistructural')]</t>
         </is>
       </c>
     </row>
@@ -3279,7 +3279,7 @@
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>[('lecture', 'Evaluating'), ('discuss', 'Understanding'), ('utilise', 'Applying'), ('assign', 'Applying'), ('validate', 'Evaluating')]</t>
+          <t>[('lecture', 'Evaluating'), ('discuss', 'Applying'), ('utilise', 'Applying'), ('assign', 'Applying'), ('validate', 'Evaluating')]</t>
         </is>
       </c>
     </row>
@@ -3294,22 +3294,22 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>SOLO</t>
+          <t>Cognitive</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>Multistructural</t>
+          <t>Analysing</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>[('determine', 'Multistructural'), ('involve', 'Verb not mapped'), ('use', 'Relational'), ('solve', 'Multistructural')]</t>
+          <t>[('determine', 'Analysing'), ('involve', 'Verb not mapped'), ('use', 'Applying'), ('solve', 'Analysing')]</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>[('reduce', 'Relational'), ('translate', 'Relational'), ('discern', 'Multistructural'), ('explain', 'Relational'), ('calculate', 'Relational')]</t>
+          <t>[('reduce', 'Evaluating'), ('extract', 'Analysing'), ('interface', 'Evaluating'), ('file', 'Analysing'), ('example', 'Understanding')]</t>
         </is>
       </c>
     </row>
@@ -3329,17 +3329,17 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>Creating</t>
+          <t>Evaluating</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>[('propose', 'Creating'), ('solve', 'Applying'), ('justify', 'Creating'), ('finalise', 'Verb not mapped')]</t>
+          <t>[('propose', 'Evaluating'), ('solve', 'Analysing'), ('justify', 'Evaluating'), ('finalise', 'Verb not mapped')]</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>[('produce', 'Creating'), ('monitor', 'Evaluating'), ('improve', 'Evaluating'), ('create', 'Creating'), ('adopt', 'Evaluating')]</t>
+          <t>[('mitigate', 'Creating'), ('produce', 'Creating'), ('monitor', 'Evaluating'), ('improve', 'Evaluating'), ('create', 'Creating')]</t>
         </is>
       </c>
     </row>
@@ -3354,22 +3354,22 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>SOLO</t>
+          <t>Psychomotor</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>Extended Abstract</t>
+          <t>Origination</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>[('identify', 'Unistructural'), ('develop', 'Extended Abstract'), ('validate', 'Extended Abstract'), ('convey', 'Verb not mapped')]</t>
+          <t>[('identify', 'Perception'), ('develop', 'Origination'), ('validate', 'Origination'), ('convey', 'Verb not mapped')]</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>[('generate', 'Extended Abstract'), ('validate', 'Extended Abstract'), ('value', 'Extended Abstract'), ('mitigate', 'Extended Abstract'), ('sequence', 'Multistructural')]</t>
+          <t>[('generate', 'Origination'), ('validate', 'Origination'), ('value', 'Origination'), ('trace', 'Guided Response'), ('mitigate', 'Origination')]</t>
         </is>
       </c>
     </row>
@@ -3399,7 +3399,7 @@
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>[('conduct', 'Applying'), ('reflect', 'Evaluating'), ('identify', 'Understanding'), ('factor', 'Understanding'), ('determine', 'Analysing')]</t>
+          <t>[('conduct', 'Analysing'), ('reflect', 'Evaluating'), ('identify', 'Understanding'), ('factor', 'Understanding'), ('satisfy', 'Evaluating')]</t>
         </is>
       </c>
     </row>
@@ -3414,22 +3414,22 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>SOLO</t>
+          <t>Cognitive</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>Multistructural</t>
+          <t>Analysing</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>[('discern', 'Multistructural'), ('propose', 'Multistructural')]</t>
+          <t>[('discern', 'Analysing'), ('propose', 'Evaluating')]</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>[('summarise', 'Relational'), ('apply', 'Relational'), ('calculate', 'Relational'), ('design', 'Extended Abstract'), ('derive', 'Relational')]</t>
+          <t>[('summarise', 'Applying'), ('improve', 'Evaluating'), ('investigate', 'Analysing'), ('research', 'Analysing'), ('change', 'Analysing')]</t>
         </is>
       </c>
     </row>
@@ -3459,7 +3459,7 @@
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>[('extract', 'Analysing'), ('interface', 'Evaluating'), ('file', 'Analysing'), ('example', 'Understanding'), ('trace', 'Remembering')]</t>
+          <t>[('reduce', 'Evaluating'), ('extract', 'Analysing'), ('interface', 'Evaluating'), ('file', 'Analysing'), ('example', 'Understanding')]</t>
         </is>
       </c>
     </row>
@@ -3489,7 +3489,7 @@
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>[('factor', 'Understanding'), ('integrate', 'Evaluating'), ('review', 'Remembering'), ('plan', 'Creating'), ('devise', 'Evaluating')]</t>
+          <t>[('factor', 'Understanding'), ('integrate', 'Evaluating'), ('review', 'Analysing'), ('plan', 'Creating'), ('devise', 'Evaluating')]</t>
         </is>
       </c>
     </row>
@@ -3504,22 +3504,22 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>SOLO</t>
+          <t>Psychomotor</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>Multistructural</t>
+          <t>Guided Response</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>[('determine', 'Multistructural'), ('include', 'Verb not mapped'), ('embody', 'Verb not mapped'), ('propose', 'Multistructural'), ('use', 'Relational')]</t>
+          <t>[('determine', 'Mechanism'), ('include', 'Verb not mapped'), ('embody', 'Verb not mapped'), ('propose', 'Adaptation'), ('use', 'Guided Response')]</t>
         </is>
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>[('reduce', 'Relational'), ('construct', 'Relational'), ('translate', 'Relational'), ('discern', 'Multistructural'), ('explain', 'Relational')]</t>
+          <t>[('reduce', 'Adaptation'), ('trace', 'Guided Response'), ('construct', 'Adaptation'), ('translate', 'Guided Response'), ('discern', 'Mechanism')]</t>
         </is>
       </c>
     </row>
@@ -3534,22 +3534,22 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>Cognitive</t>
+          <t>Affective</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>Applying</t>
+          <t>Valuing</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>[('discern', 'Verb not mapped'), ('work', 'Verb not mapped'), ('demonstrate', 'Applying'), ('establish', 'Applying')]</t>
+          <t>[('discern', 'Valuing'), ('work', 'Valuing'), ('demonstrate', 'Responding'), ('establish', 'Valuing')]</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>[('define', 'Remembering'), ('discuss', 'Understanding'), ('interface', 'Evaluating'), ('sequence', 'Applying'), ('produce', 'Creating')]</t>
+          <t>[('define', 'Responding'), ('guide', 'Valuing'), ('discuss', 'Responding'), ('sequence', 'Valuing'), ('deliberate', 'Characterisation')]</t>
         </is>
       </c>
     </row>
@@ -3569,17 +3569,17 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>Understanding</t>
+          <t>Applying</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>[('describe', 'Understanding')]</t>
+          <t>[('describe', 'Applying')]</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>[('lecture', 'Evaluating'), ('interface', 'Evaluating'), ('simulate', 'Applying'), ('produce', 'Creating'), ('trace', 'Remembering')]</t>
+          <t>[('lecture', 'Evaluating'), ('interface', 'Evaluating'), ('simulate', 'Analysing'), ('produce', 'Creating'), ('trace', 'Remembering')]</t>
         </is>
       </c>
     </row>
@@ -3594,22 +3594,22 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>SOLO</t>
+          <t>Cognitive</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>Multistructural</t>
+          <t>Applying</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>[('describe', 'Multistructural'), ('define', 'Multistructural'), ('discern', 'Multistructural'), ('lead', 'Verb not mapped')]</t>
+          <t>[('describe', 'Applying'), ('define', 'Applying'), ('discern', 'Analysing'), ('lead', 'Verb not mapped')]</t>
         </is>
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>[('compare', 'Relational'), ('satisfy', 'Relational'), ('value', 'Extended Abstract'), ('generate', 'Extended Abstract'), ('define', 'Multistructural')]</t>
+          <t>[('assign', 'Applying'), ('compare', 'Applying'), ('lecture', 'Evaluating'), ('act', 'Analysing'), ('satisfy', 'Evaluating')]</t>
         </is>
       </c>
     </row>
@@ -3629,17 +3629,17 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>Understanding</t>
+          <t>Applying</t>
         </is>
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>[('discuss', 'Understanding'), ('integrate', 'Evaluating')]</t>
+          <t>[('discuss', 'Applying'), ('integrate', 'Evaluating')]</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>[('back', 'Applying'), ('trace', 'Remembering'), ('discuss', 'Understanding'), ('integrate', 'Evaluating'), ('lecture', 'Evaluating')]</t>
+          <t>[('back', 'Applying'), ('trace', 'Remembering'), ('discuss', 'Applying'), ('integrate', 'Evaluating'), ('lecture', 'Evaluating')]</t>
         </is>
       </c>
     </row>
@@ -3654,22 +3654,22 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>SOLO</t>
+          <t>Cognitive</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>Multistructural</t>
+          <t>Applying</t>
         </is>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>[('define', 'Multistructural'), ('use', 'Relational'), ('discern', 'Multistructural'), ('solve', 'Multistructural'), ('decompose', 'Verb not mapped'), ('use', 'Relational'), ('describe', 'Multistructural')]</t>
+          <t>[('define', 'Applying'), ('use', 'Applying'), ('discern', 'Analysing'), ('solve', 'Analysing'), ('decompose', 'Verb not mapped'), ('use', 'Applying'), ('describe', 'Applying')]</t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>[('simulate', 'Extended Abstract'), ('discern', 'Multistructural'), ('appreciate', 'Relational'), ('translate', 'Relational'), ('characterise', 'Relational')]</t>
+          <t>[('lecture', 'Evaluating'), ('interface', 'Evaluating'), ('simulate', 'Analysing'), ('produce', 'Creating'), ('trace', 'Remembering')]</t>
         </is>
       </c>
     </row>
@@ -3699,7 +3699,7 @@
       </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t>[('order', 'Unistructural'), ('compute', 'Relational'), ('derive', 'Relational'), ('summarise', 'Relational'), ('create', 'Extended Abstract')]</t>
+          <t>[('order', 'Unistructural'), ('compute', 'Multistructural'), ('derive', 'Multistructural'), ('summarise', 'Unistructural'), ('create', 'Extended Abstract')]</t>
         </is>
       </c>
     </row>
@@ -3719,17 +3719,17 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>Understanding</t>
+          <t>Evaluating</t>
         </is>
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>[('propose', 'Creating'), ('give', 'Understanding'), ('evaluate', 'Evaluating')]</t>
+          <t>[('propose', 'Evaluating'), ('give', 'Understanding'), ('evaluate', 'Evaluating')]</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
         <is>
-          <t>[('experiment', 'Analysing'), ('compare', 'Understanding'), ('file', 'Analysing'), ('respond', 'Understanding'), ('document', 'Analysing')]</t>
+          <t>[('experiment', 'Analysing'), ('compare', 'Applying'), ('file', 'Analysing'), ('respond', 'Understanding'), ('document', 'Analysing')]</t>
         </is>
       </c>
     </row>
@@ -3744,22 +3744,22 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>SOLO</t>
+          <t>Psychomotor</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>Extended Abstract</t>
+          <t>Origination</t>
         </is>
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>[('identify', 'Unistructural'), ('develop', 'Extended Abstract'), ('validate', 'Extended Abstract')]</t>
+          <t>[('identify', 'Perception'), ('develop', 'Origination'), ('validate', 'Origination')]</t>
         </is>
       </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t>[('calculate', 'Relational'), ('generate', 'Extended Abstract'), ('define', 'Multistructural'), ('integrate', 'Extended Abstract'), ('compare', 'Relational')]</t>
+          <t>[('trace', 'Guided Response'), ('calculate', 'Mechanism'), ('generate', 'Origination'), ('define', 'Guided Response'), ('prepare', 'Guided Response')]</t>
         </is>
       </c>
     </row>
@@ -3789,7 +3789,7 @@
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t>[('adopt', 'Evaluating'), ('monitor', 'Evaluating'), ('devise', 'Evaluating'), ('assess', 'Evaluating'), ('experiment', 'Analysing')]</t>
+          <t>[('mitigate', 'Creating'), ('adopt', 'Evaluating'), ('address', 'Evaluating'), ('monitor', 'Evaluating'), ('devise', 'Evaluating')]</t>
         </is>
       </c>
     </row>
@@ -3809,17 +3809,17 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>Understanding</t>
+          <t>Applying</t>
         </is>
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>[('describe', 'Understanding')]</t>
+          <t>[('describe', 'Applying')]</t>
         </is>
       </c>
       <c r="F112" t="inlineStr">
         <is>
-          <t>[('lecture', 'Evaluating'), ('interface', 'Evaluating'), ('simulate', 'Applying'), ('produce', 'Creating'), ('trace', 'Remembering')]</t>
+          <t>[('lecture', 'Evaluating'), ('interface', 'Evaluating'), ('simulate', 'Analysing'), ('produce', 'Creating'), ('trace', 'Remembering')]</t>
         </is>
       </c>
     </row>
@@ -3849,7 +3849,7 @@
       </c>
       <c r="F113" t="inlineStr">
         <is>
-          <t>[('conduct', 'Applying'), ('reflect', 'Evaluating'), ('identify', 'Understanding'), ('factor', 'Understanding'), ('determine', 'Analysing')]</t>
+          <t>[('conduct', 'Analysing'), ('reflect', 'Evaluating'), ('identify', 'Understanding'), ('factor', 'Understanding'), ('satisfy', 'Evaluating')]</t>
         </is>
       </c>
     </row>
@@ -3869,17 +3869,17 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>Applying</t>
+          <t>Analysing</t>
         </is>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>[('analyse', 'Analysing'), ('apply', 'Applying'), ('solve', 'Applying')]</t>
+          <t>[('analyse', 'Analysing'), ('apply', 'Analysing'), ('solve', 'Analysing')]</t>
         </is>
       </c>
       <c r="F114" t="inlineStr">
         <is>
-          <t>[('query', 'Analysing'), ('interface', 'Evaluating'), ('describe', 'Understanding'), ('group', 'Analysing'), ('generate', 'Creating')]</t>
+          <t>[('query', 'Analysing'), ('interface', 'Evaluating'), ('describe', 'Applying'), ('group', 'Analysing'), ('generate', 'Creating')]</t>
         </is>
       </c>
     </row>
@@ -3894,22 +3894,22 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>SOLO</t>
+          <t>Affective</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>Relational</t>
+          <t>Organisation</t>
         </is>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>[('prove', 'Relational'), ('analyse', 'Relational')]</t>
+          <t>[('prove', 'Organisation'), ('analyse', 'Organisation')]</t>
         </is>
       </c>
       <c r="F115" t="inlineStr">
         <is>
-          <t>[('function', 'Relational'), ('derive', 'Relational'), ('compare', 'Relational'), ('compute', 'Relational'), ('order', 'Unistructural')]</t>
+          <t>[('complete', 'Valuing'), ('function', 'Characterisation'), ('change', 'Valuing'), ('derive', 'Valuing'), ('compare', 'Responding')]</t>
         </is>
       </c>
     </row>
@@ -3924,22 +3924,22 @@
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>SOLO</t>
+          <t>Affective</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>Relational</t>
+          <t>Responding</t>
         </is>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>[('compare', 'Relational'), ('contrast', 'Relational'), ('use', 'Relational')]</t>
+          <t>[('compare', 'Responding'), ('contrast', 'Organisation'), ('use', 'Responding')]</t>
         </is>
       </c>
       <c r="F116" t="inlineStr">
         <is>
-          <t>[('reduce', 'Relational'), ('construct', 'Relational'), ('translate', 'Relational'), ('discern', 'Multistructural'), ('explain', 'Relational')]</t>
+          <t>[('reduce', 'Organisation'), ('construct', 'Organisation'), ('translate', 'Responding'), ('discern', 'Valuing'), ('explain', 'Responding')]</t>
         </is>
       </c>
     </row>
@@ -3959,17 +3959,17 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>Applying</t>
+          <t>Analysing</t>
         </is>
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>[('develop', 'Creating'), ('implement', 'Applying'), ('solve', 'Applying')]</t>
+          <t>[('develop', 'Creating'), ('implement', 'Analysing'), ('solve', 'Analysing')]</t>
         </is>
       </c>
       <c r="F117" t="inlineStr">
         <is>
-          <t>[('debug', 'Evaluating'), ('interpret', 'Applying'), ('analyse', 'Analysing'), ('example', 'Understanding'), ('use', 'Applying')]</t>
+          <t>[('function', 'Evaluating'), ('debug', 'Evaluating'), ('interpret', 'Analysing'), ('analyse', 'Analysing'), ('example', 'Understanding')]</t>
         </is>
       </c>
     </row>
@@ -3984,22 +3984,22 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>SOLO</t>
+          <t>Cognitive</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>Relational</t>
+          <t>Analysing</t>
         </is>
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>[('translate', 'Relational'), ('implement', 'Relational')]</t>
+          <t>[('translate', 'Applying'), ('implement', 'Analysing')]</t>
         </is>
       </c>
       <c r="F118" t="inlineStr">
         <is>
-          <t>[('function', 'Relational'), ('engage', 'Extended Abstract'), ('report', 'Multistructural'), ('identify', 'Unistructural'), ('review', 'Extended Abstract')]</t>
+          <t>[('function', 'Evaluating'), ('engage', 'Creating'), ('report', 'Applying'), ('identify', 'Understanding'), ('review', 'Analysing')]</t>
         </is>
       </c>
     </row>
@@ -4029,7 +4029,7 @@
       </c>
       <c r="F119" t="inlineStr">
         <is>
-          <t>[('factor', 'Understanding'), ('integrate', 'Evaluating'), ('review', 'Remembering'), ('plan', 'Creating'), ('devise', 'Evaluating')]</t>
+          <t>[('factor', 'Understanding'), ('integrate', 'Evaluating'), ('review', 'Analysing'), ('plan', 'Creating'), ('devise', 'Evaluating')]</t>
         </is>
       </c>
     </row>
@@ -4059,7 +4059,7 @@
       </c>
       <c r="F120" t="inlineStr">
         <is>
-          <t>[('experiment', 'Analysing'), ('compare', 'Understanding'), ('file', 'Analysing'), ('respond', 'Understanding'), ('document', 'Analysing')]</t>
+          <t>[('experiment', 'Analysing'), ('compare', 'Applying'), ('file', 'Analysing'), ('respond', 'Understanding'), ('document', 'Analysing')]</t>
         </is>
       </c>
     </row>
@@ -4089,7 +4089,7 @@
       </c>
       <c r="F121" t="inlineStr">
         <is>
-          <t>[('contrast', 'Analysing'), ('define', 'Remembering'), ('interface', 'Evaluating'), ('compare', 'Understanding'), ('lecture', 'Evaluating')]</t>
+          <t>[('mitigate', 'Creating'), ('contrast', 'Analysing'), ('define', 'Applying'), ('interface', 'Evaluating'), ('compare', 'Applying')]</t>
         </is>
       </c>
     </row>
@@ -4104,22 +4104,22 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>Cognitive</t>
+          <t>Psychomotor</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>Applying</t>
+          <t>Guided Response</t>
         </is>
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>[('work', 'Verb not mapped'), ('analyse', 'Analysing'), ('write', 'Applying')]</t>
+          <t>[('work', 'Guided Response'), ('analyse', 'Adaptation'), ('write', 'Guided Response')]</t>
         </is>
       </c>
       <c r="F122" t="inlineStr">
         <is>
-          <t>[('detail', 'Understanding'), ('generate', 'Creating'), ('prepare', 'Applying'), ('report', 'Understanding'), ('query', 'Analysing')]</t>
+          <t>[('generate', 'Origination'), ('prepare', 'Guided Response'), ('report', 'Guided Response'), ('reduce', 'Adaptation'), ('engage', 'Origination')]</t>
         </is>
       </c>
     </row>
@@ -4139,17 +4139,17 @@
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>Applying</t>
+          <t>Analysing</t>
         </is>
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>[('apply', 'Applying'), ('orient', 'Verb not mapped'), ('design', 'Creating'), ('use', 'Applying')]</t>
+          <t>[('apply', 'Analysing'), ('orient', 'Verb not mapped'), ('design', 'Creating'), ('use', 'Applying')]</t>
         </is>
       </c>
       <c r="F123" t="inlineStr">
         <is>
-          <t>[('extract', 'Analysing'), ('interface', 'Evaluating'), ('file', 'Analysing'), ('example', 'Understanding'), ('trace', 'Remembering')]</t>
+          <t>[('reduce', 'Evaluating'), ('extract', 'Analysing'), ('interface', 'Evaluating'), ('file', 'Analysing'), ('example', 'Understanding')]</t>
         </is>
       </c>
     </row>
@@ -4179,7 +4179,7 @@
       </c>
       <c r="F124" t="inlineStr">
         <is>
-          <t>[('query', 'Valuing'), ('agree', 'Responding'), ('follow', 'Receiving'), ('generate', 'Organisation'), ('prepare', 'Organisation')]</t>
+          <t>[('query', 'Valuing'), ('agree', 'Responding'), ('follow', 'Receiving'), ('generate', 'Organisation'), ('prepare', 'Responding')]</t>
         </is>
       </c>
     </row>
@@ -4199,17 +4199,17 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>Applying</t>
+          <t>Analysing</t>
         </is>
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>[('apply', 'Applying'), ('orient', 'Verb not mapped'), ('implement', 'Applying'), ('orient', 'Verb not mapped'), ('use', 'Applying')]</t>
+          <t>[('apply', 'Analysing'), ('orient', 'Verb not mapped'), ('implement', 'Analysing'), ('orient', 'Verb not mapped'), ('use', 'Applying')]</t>
         </is>
       </c>
       <c r="F125" t="inlineStr">
         <is>
-          <t>[('extract', 'Analysing'), ('interface', 'Evaluating'), ('file', 'Analysing'), ('example', 'Understanding'), ('trace', 'Remembering')]</t>
+          <t>[('reduce', 'Evaluating'), ('extract', 'Analysing'), ('interface', 'Evaluating'), ('file', 'Analysing'), ('example', 'Understanding')]</t>
         </is>
       </c>
     </row>
@@ -4229,17 +4229,17 @@
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>Applying</t>
+          <t>Evaluating</t>
         </is>
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>[('apply', 'Applying'), ('refactor', 'Verb not mapped'), ('debug', 'Evaluating'), ('orient', 'Verb not mapped'), ('use', 'Applying')]</t>
+          <t>[('apply', 'Analysing'), ('refactor', 'Verb not mapped'), ('debug', 'Evaluating'), ('orient', 'Verb not mapped'), ('use', 'Applying')]</t>
         </is>
       </c>
       <c r="F126" t="inlineStr">
         <is>
-          <t>[('extract', 'Analysing'), ('interface', 'Evaluating'), ('file', 'Analysing'), ('example', 'Understanding'), ('trace', 'Remembering')]</t>
+          <t>[('reduce', 'Evaluating'), ('extract', 'Analysing'), ('interface', 'Evaluating'), ('file', 'Analysing'), ('example', 'Understanding')]</t>
         </is>
       </c>
     </row>
@@ -4254,22 +4254,22 @@
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>Cognitive</t>
+          <t>Psychomotor</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>Applying</t>
+          <t>Origination</t>
         </is>
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>[('apply', 'Applying'), ('create', 'Creating'), ('orient', 'Verb not mapped'), ('use', 'Applying'), ('include', 'Verb not mapped'), ('integrate', 'Evaluating')]</t>
+          <t>[('apply', 'Mechanism'), ('create', 'Origination'), ('orient', 'Verb not mapped'), ('use', 'Guided Response'), ('include', 'Verb not mapped'), ('integrate', 'Origination')]</t>
         </is>
       </c>
       <c r="F127" t="inlineStr">
         <is>
-          <t>[('back', 'Applying'), ('trace', 'Remembering'), ('discuss', 'Understanding'), ('lecture', 'Evaluating'), ('act', 'Applying')]</t>
+          <t>[('trace', 'Guided Response'), ('discuss', 'Guided Response'), ('follow', 'Guided Response'), ('define', 'Guided Response'), ('synthesise', 'Origination')]</t>
         </is>
       </c>
     </row>
@@ -4284,22 +4284,22 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>Affective</t>
+          <t>Cognitive</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>Receiving</t>
+          <t>Understanding</t>
         </is>
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>[('identify', 'Receiving'), ('include', 'Verb not mapped'), ('select', 'Receiving'), ('give', 'Receiving'), ('achieve', 'Verb not mapped'), ('document', 'Verb not mapped')]</t>
+          <t>[('identify', 'Understanding'), ('include', 'Verb not mapped'), ('select', 'Applying'), ('give', 'Understanding'), ('achieve', 'Verb not mapped'), ('document', 'Analysing')]</t>
         </is>
       </c>
       <c r="F128" t="inlineStr">
         <is>
-          <t>[('adopt', 'Valuing'), ('monitor', 'Valuing'), ('respond', 'Responding'), ('generate', 'Organisation'), ('prepare', 'Organisation')]</t>
+          <t>[('adopt', 'Evaluating'), ('monitor', 'Evaluating'), ('respond', 'Understanding'), ('interface', 'Evaluating'), ('generate', 'Creating')]</t>
         </is>
       </c>
     </row>
@@ -4319,17 +4319,17 @@
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>Applying</t>
+          <t>Analysing</t>
         </is>
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>[('apply', 'Applying')]</t>
+          <t>[('apply', 'Analysing')]</t>
         </is>
       </c>
       <c r="F129" t="inlineStr">
         <is>
-          <t>[('create', 'Creating'), ('summarise', 'Understanding'), ('derive', 'Applying'), ('query', 'Analysing'), ('order', 'Remembering')]</t>
+          <t>[('create', 'Creating'), ('summarise', 'Applying'), ('derive', 'Analysing'), ('query', 'Analysing'), ('order', 'Applying')]</t>
         </is>
       </c>
     </row>
@@ -4359,7 +4359,7 @@
       </c>
       <c r="F130" t="inlineStr">
         <is>
-          <t>[('factor', 'Understanding'), ('integrate', 'Evaluating'), ('review', 'Remembering'), ('plan', 'Creating'), ('devise', 'Evaluating')]</t>
+          <t>[('factor', 'Understanding'), ('integrate', 'Evaluating'), ('review', 'Analysing'), ('plan', 'Creating'), ('devise', 'Evaluating')]</t>
         </is>
       </c>
     </row>
@@ -4374,22 +4374,22 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>SOLO</t>
+          <t>Psychomotor</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>Relational</t>
+          <t>Guided Response</t>
         </is>
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>[('perform', 'Relational'), ('use', 'Relational'), ('trace', 'Verb not mapped')]</t>
+          <t>[('perform', 'Complex Overt Response'), ('use', 'Guided Response'), ('trace', 'Guided Response')]</t>
         </is>
       </c>
       <c r="F131" t="inlineStr">
         <is>
-          <t>[('perform', 'Relational'), ('mitigate', 'Extended Abstract'), ('sequence', 'Multistructural'), ('define', 'Multistructural'), ('transfer', 'Relational')]</t>
+          <t>[('perform', 'Complex Overt Response'), ('mitigate', 'Origination'), ('respond', 'Guided Response'), ('heat', 'Mechanism'), ('sequence', 'Mechanism')]</t>
         </is>
       </c>
     </row>
@@ -4414,12 +4414,12 @@
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>[('select', 'Evaluating'), ('collect', 'Applying'), ('include', 'Verb not mapped'), ('analyse', 'Analysing'), ('make', 'Creating'), ('base', 'Verb not mapped')]</t>
+          <t>[('select', 'Applying'), ('collect', 'Applying'), ('include', 'Verb not mapped'), ('analyse', 'Analysing'), ('make', 'Creating'), ('base', 'Verb not mapped')]</t>
         </is>
       </c>
       <c r="F132" t="inlineStr">
         <is>
-          <t>[('appraise', 'Evaluating'), ('conclude', 'Creating'), ('interpret', 'Applying'), ('summarise', 'Understanding'), ('group', 'Analysing')]</t>
+          <t>[('appraise', 'Evaluating'), ('conclude', 'Creating'), ('interpret', 'Analysing'), ('summarise', 'Applying'), ('partition', 'Evaluating')]</t>
         </is>
       </c>
     </row>
@@ -4449,7 +4449,7 @@
       </c>
       <c r="F133" t="inlineStr">
         <is>
-          <t>[('extract', 'Analysing'), ('interface', 'Evaluating'), ('file', 'Analysing'), ('example', 'Understanding'), ('trace', 'Remembering')]</t>
+          <t>[('reduce', 'Evaluating'), ('extract', 'Analysing'), ('interface', 'Evaluating'), ('file', 'Analysing'), ('example', 'Understanding')]</t>
         </is>
       </c>
     </row>
@@ -4464,22 +4464,22 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>Cognitive</t>
+          <t>Affective</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>Creating</t>
+          <t>Organisation</t>
         </is>
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>[('analyse', 'Analysing'), ('design', 'Creating'), ('refactor', 'Verb not mapped'), ('take', 'Verb not mapped')]</t>
+          <t>[('analyse', 'Organisation'), ('design', 'Organisation'), ('refactor', 'Verb not mapped'), ('take', 'Verb not mapped')]</t>
         </is>
       </c>
       <c r="F134" t="inlineStr">
         <is>
-          <t>[('back', 'Applying'), ('trace', 'Remembering'), ('perform', 'Creating'), ('utilise', 'Applying'), ('lecture', 'Evaluating')]</t>
+          <t>[('perform', 'Characterisation'), ('follow', 'Receiving'), ('mitigate', 'Characterisation'), ('compare', 'Responding'), ('agree', 'Responding')]</t>
         </is>
       </c>
     </row>
@@ -4504,12 +4504,12 @@
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>[('take', 'Verb not mapped'), ('develop', 'Verb not mapped'), ('follow', 'Guided Response'), ('orient', 'Verb not mapped')]</t>
+          <t>[('take', 'Verb not mapped'), ('develop', 'Origination'), ('follow', 'Guided Response'), ('orient', 'Verb not mapped')]</t>
         </is>
       </c>
       <c r="F135" t="inlineStr">
         <is>
-          <t>[('trace', 'Guided Response'), ('perform', 'Complex Overt Response'), ('respond', 'Guided Response'), ('change', 'Adaptation'), ('prepare', 'Set')]</t>
+          <t>[('characterise', 'Guided Response'), ('trace', 'Guided Response'), ('compare', 'Guided Response'), ('mitigate', 'Origination'), ('perform', 'Complex Overt Response')]</t>
         </is>
       </c>
     </row>
@@ -4524,22 +4524,22 @@
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>Affective</t>
+          <t>Cognitive</t>
         </is>
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>Receiving</t>
+          <t>Applying</t>
         </is>
       </c>
       <c r="E136" t="inlineStr">
         <is>
-          <t>[('select', 'Receiving'), ('use', 'Receiving'), ('incremente', 'Verb not mapped')]</t>
+          <t>[('select', 'Applying'), ('use', 'Applying'), ('incremente', 'Verb not mapped')]</t>
         </is>
       </c>
       <c r="F136" t="inlineStr">
         <is>
-          <t>[('relay', 'Responding'), ('study', 'Valuing'), ('consider', 'Organisation'), ('perform', 'Characterisation'), ('evaluate', 'Valuing')]</t>
+          <t>[('lecture', 'Evaluating'), ('study', 'Applying'), ('trace', 'Remembering'), ('produce', 'Creating'), ('consider', 'Evaluating')]</t>
         </is>
       </c>
     </row>
@@ -4554,22 +4554,22 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>SOLO</t>
+          <t>Affective</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>Extended Abstract</t>
+          <t>Organisation</t>
         </is>
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>[('evaluate', 'Extended Abstract'), ('apply', 'Relational'), ('design', 'Extended Abstract')]</t>
+          <t>[('evaluate', 'Organisation'), ('apply', 'Valuing'), ('design', 'Organisation')]</t>
         </is>
       </c>
       <c r="F137" t="inlineStr">
         <is>
-          <t>[('summarise', 'Relational'), ('order', 'Unistructural'), ('propose', 'Multistructural'), ('apply', 'Relational'), ('design', 'Extended Abstract')]</t>
+          <t>[('summarise', 'Responding'), ('order', 'Responding'), ('propose', 'Characterisation'), ('design', 'Organisation'), ('apply', 'Valuing')]</t>
         </is>
       </c>
     </row>
@@ -4589,17 +4589,17 @@
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>Creating</t>
+          <t>Evaluating</t>
         </is>
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>[('justify', 'Creating'), ('communicate', 'Verb not mapped')]</t>
+          <t>[('justify', 'Evaluating'), ('communicate', 'Verb not mapped')]</t>
         </is>
       </c>
       <c r="F138" t="inlineStr">
         <is>
-          <t>[('document', 'Analysing'), ('characterise', 'Understanding'), ('comprehend', 'Understanding'), ('identify', 'Understanding'), ('transfer', 'Applying')]</t>
+          <t>[('document', 'Analysing'), ('characterise', 'Applying'), ('comprehend', 'Understanding'), ('identify', 'Understanding'), ('transfer', 'Analysing')]</t>
         </is>
       </c>
     </row>
@@ -4629,7 +4629,7 @@
       </c>
       <c r="F139" t="inlineStr">
         <is>
-          <t>[('explore', 'Analysing'), ('complete', 'Applying'), ('rate', 'Evaluating'), ('change', 'Applying'), ('improve', 'Evaluating')]</t>
+          <t>[('explore', 'Analysing'), ('complete', 'Applying'), ('function', 'Evaluating'), ('rate', 'Evaluating'), ('change', 'Analysing')]</t>
         </is>
       </c>
     </row>
@@ -4644,22 +4644,22 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>SOLO</t>
+          <t>Cognitive</t>
         </is>
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>Relational</t>
+          <t>Applying</t>
         </is>
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>[('explain', 'Relational'), ('analyse', 'Relational')]</t>
+          <t>[('explain', 'Applying'), ('analyse', 'Analysing')]</t>
         </is>
       </c>
       <c r="F140" t="inlineStr">
         <is>
-          <t>[('function', 'Relational'), ('derive', 'Relational'), ('compare', 'Relational'), ('compute', 'Relational'), ('order', 'Unistructural')]</t>
+          <t>[('explore', 'Analysing'), ('complete', 'Applying'), ('function', 'Evaluating'), ('rate', 'Evaluating'), ('change', 'Analysing')]</t>
         </is>
       </c>
     </row>
@@ -4674,22 +4674,22 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>SOLO</t>
+          <t>Cognitive</t>
         </is>
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>Relational</t>
+          <t>Applying</t>
         </is>
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>[('explain', 'Relational'), ('analyse', 'Relational')]</t>
+          <t>[('explain', 'Applying'), ('analyse', 'Analysing')]</t>
         </is>
       </c>
       <c r="F141" t="inlineStr">
         <is>
-          <t>[('function', 'Relational'), ('derive', 'Relational'), ('compare', 'Relational'), ('compute', 'Relational'), ('order', 'Unistructural')]</t>
+          <t>[('explore', 'Analysing'), ('complete', 'Applying'), ('function', 'Evaluating'), ('rate', 'Evaluating'), ('change', 'Analysing')]</t>
         </is>
       </c>
     </row>
@@ -4719,7 +4719,7 @@
       </c>
       <c r="F142" t="inlineStr">
         <is>
-          <t>[('interface', 'Evaluating'), ('construct', 'Creating'), ('lecture', 'Evaluating'), ('complete', 'Applying'), ('trace', 'Remembering')]</t>
+          <t>[('interface', 'Evaluating'), ('reduce', 'Evaluating'), ('construct', 'Evaluating'), ('lecture', 'Evaluating'), ('complete', 'Applying')]</t>
         </is>
       </c>
     </row>
@@ -4749,7 +4749,7 @@
       </c>
       <c r="F143" t="inlineStr">
         <is>
-          <t>[('differentiate', 'Analysing'), ('specify', 'Evaluating'), ('derive', 'Applying'), ('summarise', 'Understanding'), ('example', 'Understanding')]</t>
+          <t>[('differentiate', 'Applying'), ('specify', 'Evaluating'), ('derive', 'Analysing'), ('summarise', 'Applying'), ('example', 'Understanding')]</t>
         </is>
       </c>
     </row>
@@ -4769,12 +4769,12 @@
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>Understanding</t>
+          <t>Applying</t>
         </is>
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>[('describe', 'Understanding'), ('base', 'Verb not mapped'), ('apply', 'Applying'), ('achieve', 'Verb not mapped')]</t>
+          <t>[('describe', 'Applying'), ('base', 'Verb not mapped'), ('apply', 'Analysing'), ('achieve', 'Verb not mapped')]</t>
         </is>
       </c>
       <c r="F144" t="inlineStr">
@@ -4799,17 +4799,17 @@
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>Applying</t>
+          <t>Analysing</t>
         </is>
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>[('apply', 'Applying'), ('engage', 'Verb not mapped'), ('determine', 'Analysing')]</t>
+          <t>[('apply', 'Analysing'), ('engage', 'Creating'), ('determine', 'Analysing')]</t>
         </is>
       </c>
       <c r="F145" t="inlineStr">
         <is>
-          <t>[('contrast', 'Analysing'), ('define', 'Remembering'), ('interface', 'Evaluating'), ('compare', 'Understanding'), ('lecture', 'Evaluating')]</t>
+          <t>[('mitigate', 'Creating'), ('contrast', 'Analysing'), ('define', 'Applying'), ('interface', 'Evaluating'), ('compare', 'Applying')]</t>
         </is>
       </c>
     </row>
@@ -4864,7 +4864,7 @@
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>[('compare', 'Understanding'), ('analyse', 'Analysing'), ('determine', 'Analysing'), ('require', 'Verb not mapped'), ('support', 'Evaluating')]</t>
+          <t>[('compare', 'Applying'), ('analyse', 'Analysing'), ('determine', 'Analysing'), ('require', 'Verb not mapped'), ('support', 'Evaluating')]</t>
         </is>
       </c>
       <c r="F147" t="inlineStr">
@@ -4924,12 +4924,12 @@
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>[('deliberate', 'Verb not mapped'), ('occur', 'Verb not mapped'), ('identify', 'Understanding'), ('base', 'Verb not mapped')]</t>
+          <t>[('deliberate', 'Creating'), ('occur', 'Verb not mapped'), ('identify', 'Understanding'), ('base', 'Verb not mapped')]</t>
         </is>
       </c>
       <c r="F149" t="inlineStr">
         <is>
-          <t>[('factor', 'Understanding'), ('assess', 'Evaluating'), ('identify', 'Understanding'), ('review', 'Remembering'), ('group', 'Analysing')]</t>
+          <t>[('factor', 'Understanding'), ('assess', 'Evaluating'), ('address', 'Evaluating'), ('identify', 'Understanding'), ('review', 'Analysing')]</t>
         </is>
       </c>
     </row>
@@ -4949,17 +4949,17 @@
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>Applying</t>
+          <t>Analysing</t>
         </is>
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>[('apply', 'Applying')]</t>
+          <t>[('apply', 'Analysing')]</t>
         </is>
       </c>
       <c r="F150" t="inlineStr">
         <is>
-          <t>[('create', 'Creating'), ('summarise', 'Understanding'), ('derive', 'Applying'), ('query', 'Analysing'), ('order', 'Remembering')]</t>
+          <t>[('create', 'Creating'), ('summarise', 'Applying'), ('derive', 'Analysing'), ('query', 'Analysing'), ('order', 'Applying')]</t>
         </is>
       </c>
     </row>
@@ -4989,7 +4989,7 @@
       </c>
       <c r="F151" t="inlineStr">
         <is>
-          <t>[('validate', 'Evaluating'), ('lecture', 'Evaluating'), ('study', 'Remembering'), ('specify', 'Evaluating'), ('trace', 'Remembering')]</t>
+          <t>[('validate', 'Evaluating'), ('lecture', 'Evaluating'), ('study', 'Applying'), ('specify', 'Evaluating'), ('trace', 'Remembering')]</t>
         </is>
       </c>
     </row>
@@ -5009,17 +5009,17 @@
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>Applying</t>
+          <t>Analysing</t>
         </is>
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>[('implement', 'Applying'), ('base', 'Verb not mapped')]</t>
+          <t>[('implement', 'Analysing'), ('base', 'Verb not mapped')]</t>
         </is>
       </c>
       <c r="F152" t="inlineStr">
         <is>
-          <t>[('debug', 'Evaluating'), ('improve', 'Evaluating'), ('construct', 'Creating'), ('example', 'Understanding'), ('use', 'Applying')]</t>
+          <t>[('debug', 'Evaluating'), ('improve', 'Evaluating'), ('construct', 'Evaluating'), ('example', 'Understanding'), ('use', 'Applying')]</t>
         </is>
       </c>
     </row>
@@ -5049,7 +5049,7 @@
       </c>
       <c r="F153" t="inlineStr">
         <is>
-          <t>[('factor', 'Understanding'), ('integrate', 'Evaluating'), ('review', 'Remembering'), ('plan', 'Creating'), ('devise', 'Evaluating')]</t>
+          <t>[('factor', 'Understanding'), ('integrate', 'Evaluating'), ('review', 'Analysing'), ('plan', 'Creating'), ('devise', 'Evaluating')]</t>
         </is>
       </c>
     </row>
@@ -5069,17 +5069,17 @@
       </c>
       <c r="D154" t="inlineStr">
         <is>
-          <t>Analysing</t>
+          <t>Applying</t>
         </is>
       </c>
       <c r="E154" t="inlineStr">
         <is>
-          <t>[('differentiate', 'Analysing')]</t>
+          <t>[('differentiate', 'Applying')]</t>
         </is>
       </c>
       <c r="F154" t="inlineStr">
         <is>
-          <t>[('prepare', 'Applying'), ('generate', 'Creating'), ('sequence', 'Applying'), ('trace', 'Remembering'), ('lecture', 'Evaluating')]</t>
+          <t>[('prepare', 'Analysing'), ('generate', 'Creating'), ('sequence', 'Applying'), ('trace', 'Remembering'), ('lecture', 'Evaluating')]</t>
         </is>
       </c>
     </row>
@@ -5109,7 +5109,7 @@
       </c>
       <c r="F155" t="inlineStr">
         <is>
-          <t>[('validate', 'Evaluating'), ('lecture', 'Evaluating'), ('study', 'Remembering'), ('specify', 'Evaluating'), ('trace', 'Remembering')]</t>
+          <t>[('validate', 'Evaluating'), ('lecture', 'Evaluating'), ('study', 'Applying'), ('specify', 'Evaluating'), ('trace', 'Remembering')]</t>
         </is>
       </c>
     </row>
@@ -5129,17 +5129,17 @@
       </c>
       <c r="D156" t="inlineStr">
         <is>
-          <t>Applying</t>
+          <t>Analysing</t>
         </is>
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>[('design', 'Creating'), ('implement', 'Applying')]</t>
+          <t>[('design', 'Creating'), ('implement', 'Analysing')]</t>
         </is>
       </c>
       <c r="F156" t="inlineStr">
         <is>
-          <t>[('design', 'Creating'), ('implement', 'Applying'), ('debug', 'Evaluating'), ('analyse', 'Analysing'), ('improve', 'Evaluating')]</t>
+          <t>[('function', 'Evaluating'), ('design', 'Creating'), ('implement', 'Analysing'), ('debug', 'Evaluating'), ('analyse', 'Analysing')]</t>
         </is>
       </c>
     </row>
@@ -5154,22 +5154,22 @@
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>Affective</t>
+          <t>Cognitive</t>
         </is>
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t>Receiving</t>
+          <t>Applying</t>
         </is>
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>[('select', 'Receiving'), ('use', 'Receiving'), ('manage', 'Organisation'), ('include', 'Verb not mapped')]</t>
+          <t>[('select', 'Applying'), ('use', 'Applying'), ('manage', 'Analysing'), ('include', 'Verb not mapped')]</t>
         </is>
       </c>
       <c r="F157" t="inlineStr">
         <is>
-          <t>[('integrate', 'Organisation'), ('plan', 'Organisation'), ('discuss', 'Responding'), ('agree', 'Responding'), ('adopt', 'Valuing')]</t>
+          <t>[('factor', 'Understanding'), ('integrate', 'Evaluating'), ('review', 'Analysing'), ('plan', 'Creating'), ('devise', 'Evaluating')]</t>
         </is>
       </c>
     </row>
@@ -5194,12 +5194,12 @@
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t>[('identify', 'Understanding'), ('include', 'Verb not mapped'), ('devise', 'Evaluating'), ('adopt', 'Evaluating'), ('monitor', 'Evaluating'), ('mitigate', 'Verb not mapped')]</t>
+          <t>[('identify', 'Understanding'), ('include', 'Verb not mapped'), ('devise', 'Evaluating'), ('adopt', 'Evaluating'), ('monitor', 'Evaluating'), ('mitigate', 'Creating')]</t>
         </is>
       </c>
       <c r="F158" t="inlineStr">
         <is>
-          <t>[('monitor', 'Evaluating'), ('adopt', 'Evaluating'), ('trace', 'Remembering'), ('interface', 'Evaluating'), ('devise', 'Evaluating')]</t>
+          <t>[('mitigate', 'Creating'), ('monitor', 'Evaluating'), ('adopt', 'Evaluating'), ('trace', 'Remembering'), ('interface', 'Evaluating')]</t>
         </is>
       </c>
     </row>
@@ -5224,12 +5224,12 @@
       </c>
       <c r="E159" t="inlineStr">
         <is>
-          <t>[('choose', 'Receiving'), ('follow', 'Receiving'), ('justify', 'Valuing')]</t>
+          <t>[('choose', 'Receiving'), ('follow', 'Receiving'), ('justify', 'Organisation')]</t>
         </is>
       </c>
       <c r="F159" t="inlineStr">
         <is>
-          <t>[('adopt', 'Valuing'), ('monitor', 'Valuing'), ('collaborate', 'Organisation'), ('generate', 'Organisation'), ('report', 'Valuing')]</t>
+          <t>[('adopt', 'Valuing'), ('monitor', 'Valuing'), ('collaborate', 'Organisation'), ('generate', 'Organisation'), ('mitigate', 'Characterisation')]</t>
         </is>
       </c>
     </row>
@@ -5259,7 +5259,7 @@
       </c>
       <c r="F160" t="inlineStr">
         <is>
-          <t>[('document', 'Analysing'), ('evaluate', 'Evaluating'), ('file', 'Analysing'), ('rate', 'Evaluating'), ('characterise', 'Understanding')]</t>
+          <t>[('document', 'Analysing'), ('evaluate', 'Evaluating'), ('file', 'Analysing'), ('rate', 'Evaluating'), ('characterise', 'Applying')]</t>
         </is>
       </c>
     </row>
@@ -5284,7 +5284,7 @@
       </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t>[('produce', 'Creating'), ('support', 'Evaluating'), ('include', 'Verb not mapped'), ('address', 'Verb not mapped')]</t>
+          <t>[('produce', 'Creating'), ('support', 'Evaluating'), ('include', 'Verb not mapped'), ('address', 'Evaluating')]</t>
         </is>
       </c>
       <c r="F161" t="inlineStr">
@@ -5319,7 +5319,7 @@
       </c>
       <c r="F162" t="inlineStr">
         <is>
-          <t>[('integrate', 'Organisation'), ('plan', 'Organisation'), ('discuss', 'Responding'), ('agree', 'Responding'), ('adopt', 'Valuing')]</t>
+          <t>[('integrate', 'Organisation'), ('review', 'Valuing'), ('plan', 'Organisation'), ('discuss', 'Responding'), ('agree', 'Responding')]</t>
         </is>
       </c>
     </row>
@@ -5349,7 +5349,7 @@
       </c>
       <c r="F163" t="inlineStr">
         <is>
-          <t>[('relay', 'Responding'), ('generate', 'Organisation'), ('adopt', 'Valuing'), ('discuss', 'Responding'), ('guide', 'Valuing')]</t>
+          <t>[('relay', 'Responding'), ('mitigate', 'Characterisation'), ('generate', 'Organisation'), ('adopt', 'Valuing'), ('sequence', 'Valuing')]</t>
         </is>
       </c>
     </row>
@@ -5364,12 +5364,12 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>SOLO</t>
+          <t>Cognitive</t>
         </is>
       </c>
       <c r="D164" t="inlineStr">
         <is>
-          <t>Relational</t>
+          <t>Evaluating</t>
         </is>
       </c>
       <c r="E164" t="inlineStr">
@@ -5379,7 +5379,7 @@
       </c>
       <c r="F164" t="inlineStr">
         <is>
-          <t>[('reduce', 'Relational'), ('simulate', 'Extended Abstract'), ('mitigate', 'Extended Abstract'), ('calculate', 'Relational'), ('discuss', 'Relational')]</t>
+          <t>[('reduce', 'Evaluating'), ('file', 'Analysing'), ('interface', 'Evaluating'), ('lecture', 'Evaluating'), ('explore', 'Analysing')]</t>
         </is>
       </c>
     </row>
@@ -5409,7 +5409,7 @@
       </c>
       <c r="F165" t="inlineStr">
         <is>
-          <t>[('lecture', 'Evaluating'), ('generate', 'Creating'), ('assign', 'Applying'), ('study', 'Remembering'), ('improve', 'Evaluating')]</t>
+          <t>[('lecture', 'Evaluating'), ('generate', 'Creating'), ('assign', 'Applying'), ('mitigate', 'Creating'), ('study', 'Applying')]</t>
         </is>
       </c>
     </row>
@@ -5439,7 +5439,7 @@
       </c>
       <c r="F166" t="inlineStr">
         <is>
-          <t>[('factor', 'Understanding'), ('integrate', 'Evaluating'), ('review', 'Remembering'), ('plan', 'Creating'), ('devise', 'Evaluating')]</t>
+          <t>[('factor', 'Understanding'), ('integrate', 'Evaluating'), ('review', 'Analysing'), ('plan', 'Creating'), ('devise', 'Evaluating')]</t>
         </is>
       </c>
     </row>
@@ -5469,7 +5469,7 @@
       </c>
       <c r="F167" t="inlineStr">
         <is>
-          <t>[('extract', 'Analysing'), ('interface', 'Evaluating'), ('file', 'Analysing'), ('example', 'Understanding'), ('trace', 'Remembering')]</t>
+          <t>[('reduce', 'Evaluating'), ('extract', 'Analysing'), ('interface', 'Evaluating'), ('file', 'Analysing'), ('example', 'Understanding')]</t>
         </is>
       </c>
     </row>
@@ -5489,17 +5489,17 @@
       </c>
       <c r="D168" t="inlineStr">
         <is>
-          <t>Organisation</t>
+          <t>Responding</t>
         </is>
       </c>
       <c r="E168" t="inlineStr">
         <is>
-          <t>[('prepare', 'Organisation'), ('write', 'Responding')]</t>
+          <t>[('prepare', 'Responding'), ('write', 'Responding')]</t>
         </is>
       </c>
       <c r="F168" t="inlineStr">
         <is>
-          <t>[('generate', 'Organisation'), ('prepare', 'Organisation'), ('write', 'Responding'), ('report', 'Valuing'), ('query', 'Valuing')]</t>
+          <t>[('generate', 'Organisation'), ('prepare', 'Responding'), ('write', 'Responding'), ('report', 'Responding'), ('query', 'Valuing')]</t>
         </is>
       </c>
     </row>
@@ -5524,12 +5524,12 @@
       </c>
       <c r="E169" t="inlineStr">
         <is>
-          <t>[('address', 'Verb not mapped'), ('identify', 'Understanding'), ('assess', 'Evaluating')]</t>
+          <t>[('address', 'Evaluating'), ('identify', 'Understanding'), ('assess', 'Evaluating')]</t>
         </is>
       </c>
       <c r="F169" t="inlineStr">
         <is>
-          <t>[('experiment', 'Analysing'), ('calculate', 'Applying'), ('file', 'Analysing'), ('change', 'Applying'), ('compare', 'Understanding')]</t>
+          <t>[('experiment', 'Analysing'), ('calculate', 'Analysing'), ('file', 'Analysing'), ('change', 'Analysing'), ('compare', 'Applying')]</t>
         </is>
       </c>
     </row>
@@ -5559,7 +5559,7 @@
       </c>
       <c r="F170" t="inlineStr">
         <is>
-          <t>[('validate', 'Evaluating'), ('develop', 'Creating'), ('lecture', 'Evaluating'), ('study', 'Remembering'), ('specify', 'Evaluating')]</t>
+          <t>[('validate', 'Evaluating'), ('develop', 'Creating'), ('issue', 'Analysing'), ('lecture', 'Evaluating'), ('study', 'Applying')]</t>
         </is>
       </c>
     </row>
@@ -5579,17 +5579,17 @@
       </c>
       <c r="D171" t="inlineStr">
         <is>
-          <t>Applying</t>
+          <t>Analysing</t>
         </is>
       </c>
       <c r="E171" t="inlineStr">
         <is>
-          <t>[('apply', 'Applying')]</t>
+          <t>[('apply', 'Analysing')]</t>
         </is>
       </c>
       <c r="F171" t="inlineStr">
         <is>
-          <t>[('create', 'Creating'), ('summarise', 'Understanding'), ('derive', 'Applying'), ('query', 'Analysing'), ('order', 'Remembering')]</t>
+          <t>[('create', 'Creating'), ('summarise', 'Applying'), ('derive', 'Analysing'), ('query', 'Analysing'), ('order', 'Applying')]</t>
         </is>
       </c>
     </row>
@@ -5619,7 +5619,7 @@
       </c>
       <c r="F172" t="inlineStr">
         <is>
-          <t>[('experiment', 'Analysing'), ('group', 'Analysing'), ('investigate', 'Analysing'), ('monitor', 'Evaluating'), ('prepare', 'Applying')]</t>
+          <t>[('experiment', 'Analysing'), ('mitigate', 'Creating'), ('group', 'Analysing'), ('investigate', 'Analysing'), ('monitor', 'Evaluating')]</t>
         </is>
       </c>
     </row>
@@ -5649,7 +5649,7 @@
       </c>
       <c r="F173" t="inlineStr">
         <is>
-          <t>[('explore', 'Analysing'), ('complete', 'Applying'), ('rate', 'Evaluating'), ('change', 'Applying'), ('improve', 'Evaluating')]</t>
+          <t>[('explore', 'Analysing'), ('complete', 'Applying'), ('function', 'Evaluating'), ('rate', 'Evaluating'), ('change', 'Analysing')]</t>
         </is>
       </c>
     </row>
@@ -5664,22 +5664,22 @@
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>SOLO</t>
+          <t>Cognitive</t>
         </is>
       </c>
       <c r="D174" t="inlineStr">
         <is>
-          <t>Relational</t>
+          <t>Analysing</t>
         </is>
       </c>
       <c r="E174" t="inlineStr">
         <is>
-          <t>[('analyse', 'Relational'), ('apply', 'Relational')]</t>
+          <t>[('analyse', 'Analysing'), ('apply', 'Analysing')]</t>
         </is>
       </c>
       <c r="F174" t="inlineStr">
         <is>
-          <t>[('create', 'Extended Abstract'), ('summarise', 'Relational'), ('derive', 'Relational'), ('order', 'Unistructural'), ('compute', 'Relational')]</t>
+          <t>[('create', 'Creating'), ('summarise', 'Applying'), ('derive', 'Analysing'), ('query', 'Analysing'), ('order', 'Applying')]</t>
         </is>
       </c>
     </row>
@@ -5694,22 +5694,22 @@
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>Cognitive</t>
+          <t>Affective</t>
         </is>
       </c>
       <c r="D175" t="inlineStr">
         <is>
-          <t>Applying</t>
+          <t>Valuing</t>
         </is>
       </c>
       <c r="E175" t="inlineStr">
         <is>
-          <t>[('implement', 'Applying'), ('use', 'Applying'), ('work', 'Verb not mapped')]</t>
+          <t>[('implement', 'Valuing'), ('use', 'Responding'), ('work', 'Valuing')]</t>
         </is>
       </c>
       <c r="F175" t="inlineStr">
         <is>
-          <t>[('monitor', 'Evaluating'), ('define', 'Remembering'), ('ensure', 'Analysing'), ('act', 'Applying'), ('detail', 'Understanding')]</t>
+          <t>[('collaborate', 'Organisation'), ('satisfy', 'Organisation'), ('monitor', 'Valuing'), ('engage', 'Characterisation'), ('define', 'Responding')]</t>
         </is>
       </c>
     </row>
@@ -5739,7 +5739,7 @@
       </c>
       <c r="F176" t="inlineStr">
         <is>
-          <t>[('explore', 'Analysing'), ('complete', 'Applying'), ('rate', 'Evaluating'), ('change', 'Applying'), ('improve', 'Evaluating')]</t>
+          <t>[('explore', 'Analysing'), ('complete', 'Applying'), ('function', 'Evaluating'), ('rate', 'Evaluating'), ('change', 'Analysing')]</t>
         </is>
       </c>
     </row>
@@ -5769,7 +5769,7 @@
       </c>
       <c r="F177" t="inlineStr">
         <is>
-          <t>[('explore', 'Analysing'), ('complete', 'Applying'), ('rate', 'Evaluating'), ('change', 'Applying'), ('improve', 'Evaluating')]</t>
+          <t>[('explore', 'Analysing'), ('complete', 'Applying'), ('function', 'Evaluating'), ('rate', 'Evaluating'), ('change', 'Analysing')]</t>
         </is>
       </c>
     </row>
@@ -5784,22 +5784,22 @@
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>SOLO</t>
+          <t>Cognitive</t>
         </is>
       </c>
       <c r="D178" t="inlineStr">
         <is>
-          <t>Relational</t>
+          <t>Analysing</t>
         </is>
       </c>
       <c r="E178" t="inlineStr">
         <is>
-          <t>[('analyse', 'Relational'), ('implement', 'Relational'), ('include', 'Verb not mapped')]</t>
+          <t>[('analyse', 'Analysing'), ('implement', 'Analysing'), ('include', 'Verb not mapped')]</t>
         </is>
       </c>
       <c r="F178" t="inlineStr">
         <is>
-          <t>[('integrate', 'Extended Abstract'), ('review', 'Extended Abstract'), ('plan', 'Extended Abstract'), ('discuss', 'Relational'), ('mitigate', 'Extended Abstract')]</t>
+          <t>[('factor', 'Understanding'), ('integrate', 'Evaluating'), ('review', 'Analysing'), ('plan', 'Creating'), ('devise', 'Evaluating')]</t>
         </is>
       </c>
     </row>
@@ -5814,22 +5814,22 @@
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>SOLO</t>
+          <t>Cognitive</t>
         </is>
       </c>
       <c r="D179" t="inlineStr">
         <is>
-          <t>Relational</t>
+          <t>Analysing</t>
         </is>
       </c>
       <c r="E179" t="inlineStr">
         <is>
-          <t>[('analyse', 'Relational'), ('implement', 'Relational'), ('base', 'Verb not mapped'), ('include', 'Verb not mapped')]</t>
+          <t>[('analyse', 'Analysing'), ('implement', 'Analysing'), ('base', 'Verb not mapped'), ('include', 'Verb not mapped')]</t>
         </is>
       </c>
       <c r="F179" t="inlineStr">
         <is>
-          <t>[('integrate', 'Extended Abstract'), ('review', 'Extended Abstract'), ('plan', 'Extended Abstract'), ('discuss', 'Relational'), ('mitigate', 'Extended Abstract')]</t>
+          <t>[('factor', 'Understanding'), ('integrate', 'Evaluating'), ('review', 'Analysing'), ('plan', 'Creating'), ('devise', 'Evaluating')]</t>
         </is>
       </c>
     </row>
@@ -5849,17 +5849,17 @@
       </c>
       <c r="D180" t="inlineStr">
         <is>
-          <t>Applying</t>
+          <t>Analysing</t>
         </is>
       </c>
       <c r="E180" t="inlineStr">
         <is>
-          <t>[('implement', 'Applying'), ('evaluate', 'Evaluating'), ('base', 'Verb not mapped')]</t>
+          <t>[('implement', 'Analysing'), ('evaluate', 'Evaluating'), ('base', 'Verb not mapped')]</t>
         </is>
       </c>
       <c r="F180" t="inlineStr">
         <is>
-          <t>[('experiment', 'Analysing'), ('compare', 'Understanding'), ('file', 'Analysing'), ('respond', 'Understanding'), ('document', 'Analysing')]</t>
+          <t>[('experiment', 'Analysing'), ('compare', 'Applying'), ('file', 'Analysing'), ('respond', 'Understanding'), ('document', 'Analysing')]</t>
         </is>
       </c>
     </row>
@@ -5889,7 +5889,7 @@
       </c>
       <c r="F181" t="inlineStr">
         <is>
-          <t>[('experiment', 'Analysing'), ('compare', 'Understanding'), ('file', 'Analysing'), ('respond', 'Understanding'), ('document', 'Analysing')]</t>
+          <t>[('experiment', 'Analysing'), ('compare', 'Applying'), ('file', 'Analysing'), ('respond', 'Understanding'), ('document', 'Analysing')]</t>
         </is>
       </c>
     </row>
@@ -5904,22 +5904,22 @@
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>Cognitive</t>
+          <t>Affective</t>
         </is>
       </c>
       <c r="D182" t="inlineStr">
         <is>
-          <t>Analysing</t>
+          <t>Organisation</t>
         </is>
       </c>
       <c r="E182" t="inlineStr">
         <is>
-          <t>[('analyse', 'Analysing'), ('evaluate', 'Evaluating')]</t>
+          <t>[('analyse', 'Organisation'), ('evaluate', 'Organisation')]</t>
         </is>
       </c>
       <c r="F182" t="inlineStr">
         <is>
-          <t>[('experiment', 'Analysing'), ('compare', 'Understanding'), ('file', 'Analysing'), ('respond', 'Understanding'), ('document', 'Analysing')]</t>
+          <t>[('compare', 'Responding'), ('respond', 'Responding'), ('prepare', 'Responding'), ('adopt', 'Valuing'), ('mitigate', 'Characterisation')]</t>
         </is>
       </c>
     </row>
@@ -5949,7 +5949,7 @@
       </c>
       <c r="F183" t="inlineStr">
         <is>
-          <t>[('extract', 'Analysing'), ('interface', 'Evaluating'), ('file', 'Analysing'), ('example', 'Understanding'), ('trace', 'Remembering')]</t>
+          <t>[('reduce', 'Evaluating'), ('extract', 'Analysing'), ('interface', 'Evaluating'), ('file', 'Analysing'), ('example', 'Understanding')]</t>
         </is>
       </c>
     </row>
@@ -5969,17 +5969,17 @@
       </c>
       <c r="D184" t="inlineStr">
         <is>
-          <t>Applying</t>
+          <t>Analysing</t>
         </is>
       </c>
       <c r="E184" t="inlineStr">
         <is>
-          <t>[('integrate', 'Evaluating'), ('solve', 'Applying')]</t>
+          <t>[('integrate', 'Evaluating'), ('solve', 'Analysing')]</t>
         </is>
       </c>
       <c r="F184" t="inlineStr">
         <is>
-          <t>[('back', 'Applying'), ('trace', 'Remembering'), ('discuss', 'Understanding'), ('act', 'Applying'), ('define', 'Remembering')]</t>
+          <t>[('back', 'Applying'), ('trace', 'Remembering'), ('discuss', 'Applying'), ('act', 'Analysing'), ('define', 'Applying')]</t>
         </is>
       </c>
     </row>
@@ -5999,17 +5999,17 @@
       </c>
       <c r="D185" t="inlineStr">
         <is>
-          <t>Evaluating</t>
+          <t>Analysing</t>
         </is>
       </c>
       <c r="E185" t="inlineStr">
         <is>
-          <t>[('plan', 'Creating'), ('respond', 'Understanding'), ('change', 'Applying')]</t>
+          <t>[('plan', 'Creating'), ('respond', 'Understanding'), ('change', 'Analysing')]</t>
         </is>
       </c>
       <c r="F185" t="inlineStr">
         <is>
-          <t>[('experiment', 'Analysing'), ('improve', 'Evaluating'), ('interface', 'Evaluating'), ('generate', 'Creating'), ('lecture', 'Evaluating')]</t>
+          <t>[('experiment', 'Analysing'), ('improve', 'Evaluating'), ('interface', 'Evaluating'), ('mitigate', 'Creating'), ('generate', 'Creating')]</t>
         </is>
       </c>
     </row>
@@ -6029,17 +6029,17 @@
       </c>
       <c r="D186" t="inlineStr">
         <is>
-          <t>Applying</t>
+          <t>Analysing</t>
         </is>
       </c>
       <c r="E186" t="inlineStr">
         <is>
-          <t>[('generate', 'Creating'), ('apply', 'Applying')]</t>
+          <t>[('generate', 'Creating'), ('apply', 'Analysing')]</t>
         </is>
       </c>
       <c r="F186" t="inlineStr">
         <is>
-          <t>[('create', 'Creating'), ('summarise', 'Understanding'), ('derive', 'Applying'), ('query', 'Analysing'), ('order', 'Remembering')]</t>
+          <t>[('create', 'Creating'), ('summarise', 'Applying'), ('derive', 'Analysing'), ('query', 'Analysing'), ('order', 'Applying')]</t>
         </is>
       </c>
     </row>
@@ -6064,12 +6064,12 @@
       </c>
       <c r="E187" t="inlineStr">
         <is>
-          <t>[('demonstrate', 'Valuing'), ('guide', 'Valuing'), ('include', 'Verb not mapped')]</t>
+          <t>[('demonstrate', 'Responding'), ('guide', 'Valuing'), ('include', 'Verb not mapped')]</t>
         </is>
       </c>
       <c r="F187" t="inlineStr">
         <is>
-          <t>[('integrate', 'Organisation'), ('plan', 'Organisation'), ('discuss', 'Responding'), ('agree', 'Responding'), ('adopt', 'Valuing')]</t>
+          <t>[('integrate', 'Organisation'), ('review', 'Valuing'), ('plan', 'Organisation'), ('discuss', 'Responding'), ('agree', 'Responding')]</t>
         </is>
       </c>
     </row>
@@ -6099,7 +6099,7 @@
       </c>
       <c r="F188" t="inlineStr">
         <is>
-          <t>[('factor', 'Understanding'), ('identify', 'Understanding'), ('assess', 'Evaluating'), ('review', 'Remembering'), ('group', 'Analysing')]</t>
+          <t>[('factor', 'Understanding'), ('assess', 'Evaluating'), ('identify', 'Understanding'), ('address', 'Evaluating'), ('review', 'Analysing')]</t>
         </is>
       </c>
     </row>
@@ -6129,7 +6129,7 @@
       </c>
       <c r="F189" t="inlineStr">
         <is>
-          <t>[('experiment', 'Analysing'), ('calculate', 'Applying'), ('file', 'Analysing'), ('change', 'Applying'), ('compare', 'Understanding')]</t>
+          <t>[('experiment', 'Analysing'), ('calculate', 'Analysing'), ('file', 'Analysing'), ('change', 'Analysing'), ('compare', 'Applying')]</t>
         </is>
       </c>
     </row>
@@ -6159,7 +6159,7 @@
       </c>
       <c r="F190" t="inlineStr">
         <is>
-          <t>[('factor', 'Understanding'), ('integrate', 'Evaluating'), ('review', 'Remembering'), ('plan', 'Creating'), ('devise', 'Evaluating')]</t>
+          <t>[('factor', 'Understanding'), ('integrate', 'Evaluating'), ('review', 'Analysing'), ('plan', 'Creating'), ('devise', 'Evaluating')]</t>
         </is>
       </c>
     </row>
@@ -6184,12 +6184,12 @@
       </c>
       <c r="E191" t="inlineStr">
         <is>
-          <t>[('engage', 'Verb not mapped'), ('achieve', 'Verb not mapped'), ('use', 'Applying'), ('base', 'Verb not mapped')]</t>
+          <t>[('engage', 'Creating'), ('achieve', 'Verb not mapped'), ('use', 'Applying'), ('base', 'Verb not mapped')]</t>
         </is>
       </c>
       <c r="F191" t="inlineStr">
         <is>
-          <t>[('extract', 'Analysing'), ('interface', 'Evaluating'), ('file', 'Analysing'), ('example', 'Understanding'), ('trace', 'Remembering')]</t>
+          <t>[('reduce', 'Evaluating'), ('extract', 'Analysing'), ('interface', 'Evaluating'), ('file', 'Analysing'), ('example', 'Understanding')]</t>
         </is>
       </c>
     </row>
@@ -6209,17 +6209,17 @@
       </c>
       <c r="D192" t="inlineStr">
         <is>
-          <t>Understanding</t>
+          <t>Applying</t>
         </is>
       </c>
       <c r="E192" t="inlineStr">
         <is>
-          <t>[('describe', 'Understanding'), ('underlie', 'Verb not mapped')]</t>
+          <t>[('describe', 'Applying'), ('underlie', 'Verb not mapped')]</t>
         </is>
       </c>
       <c r="F192" t="inlineStr">
         <is>
-          <t>[('trace', 'Remembering'), ('establish', 'Applying'), ('utilise', 'Applying'), ('produce', 'Creating'), ('detail', 'Understanding')]</t>
+          <t>[('trace', 'Remembering'), ('establish', 'Analysing'), ('discern', 'Analysing'), ('utilise', 'Applying'), ('produce', 'Creating')]</t>
         </is>
       </c>
     </row>
@@ -6239,17 +6239,17 @@
       </c>
       <c r="D193" t="inlineStr">
         <is>
-          <t>Understanding</t>
+          <t>Applying</t>
         </is>
       </c>
       <c r="E193" t="inlineStr">
         <is>
-          <t>[('explain', 'Understanding')]</t>
+          <t>[('explain', 'Applying')]</t>
         </is>
       </c>
       <c r="F193" t="inlineStr">
         <is>
-          <t>[('describe', 'Understanding'), ('interface', 'Evaluating'), ('lecture', 'Evaluating'), ('characterise', 'Understanding'), ('simulate', 'Applying')]</t>
+          <t>[('describe', 'Applying'), ('discern', 'Analysing'), ('interface', 'Evaluating'), ('lecture', 'Evaluating'), ('characterise', 'Applying')]</t>
         </is>
       </c>
     </row>
@@ -6269,17 +6269,17 @@
       </c>
       <c r="D194" t="inlineStr">
         <is>
-          <t>Applying</t>
+          <t>Analysing</t>
         </is>
       </c>
       <c r="E194" t="inlineStr">
         <is>
-          <t>[('implement', 'Applying')]</t>
+          <t>[('implement', 'Analysing')]</t>
         </is>
       </c>
       <c r="F194" t="inlineStr">
         <is>
-          <t>[('design', 'Creating'), ('debug', 'Evaluating'), ('analyse', 'Analysing'), ('improve', 'Evaluating'), ('construct', 'Creating')]</t>
+          <t>[('function', 'Evaluating'), ('design', 'Creating'), ('debug', 'Evaluating'), ('analyse', 'Analysing'), ('improve', 'Evaluating')]</t>
         </is>
       </c>
     </row>
@@ -6299,17 +6299,17 @@
       </c>
       <c r="D195" t="inlineStr">
         <is>
-          <t>Understanding</t>
+          <t>Applying</t>
         </is>
       </c>
       <c r="E195" t="inlineStr">
         <is>
-          <t>[('describe', 'Understanding')]</t>
+          <t>[('describe', 'Applying')]</t>
         </is>
       </c>
       <c r="F195" t="inlineStr">
         <is>
-          <t>[('lecture', 'Evaluating'), ('interface', 'Evaluating'), ('simulate', 'Applying'), ('produce', 'Creating'), ('trace', 'Remembering')]</t>
+          <t>[('lecture', 'Evaluating'), ('interface', 'Evaluating'), ('simulate', 'Analysing'), ('produce', 'Creating'), ('trace', 'Remembering')]</t>
         </is>
       </c>
     </row>
@@ -6330,17 +6330,17 @@
       </c>
       <c r="D196" t="inlineStr">
         <is>
-          <t>Applying</t>
+          <t>Analysing</t>
         </is>
       </c>
       <c r="E196" t="inlineStr">
         <is>
-          <t>[('implement', 'Applying'), ('regard', 'Verb not mapped')]</t>
+          <t>[('implement', 'Analysing'), ('regard', 'Verb not mapped')]</t>
         </is>
       </c>
       <c r="F196" t="inlineStr">
         <is>
-          <t>[('order', 'Remembering'), ('file', 'Analysing'), ('compute', 'Applying'), ('interface', 'Evaluating'), ('change', 'Applying')]</t>
+          <t>[('order', 'Applying'), ('file', 'Analysing'), ('compute', 'Analysing'), ('interface', 'Evaluating'), ('change', 'Analysing')]</t>
         </is>
       </c>
     </row>
@@ -6361,17 +6361,17 @@
       </c>
       <c r="D197" t="inlineStr">
         <is>
-          <t>Understanding</t>
+          <t>Applying</t>
         </is>
       </c>
       <c r="E197" t="inlineStr">
         <is>
-          <t>[('explain', 'Understanding')]</t>
+          <t>[('explain', 'Applying')]</t>
         </is>
       </c>
       <c r="F197" t="inlineStr">
         <is>
-          <t>[('describe', 'Understanding'), ('interface', 'Evaluating'), ('lecture', 'Evaluating'), ('characterise', 'Understanding'), ('simulate', 'Applying')]</t>
+          <t>[('describe', 'Applying'), ('discern', 'Analysing'), ('interface', 'Evaluating'), ('lecture', 'Evaluating'), ('characterise', 'Applying')]</t>
         </is>
       </c>
     </row>
@@ -6386,22 +6386,22 @@
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>Cognitive</t>
+          <t>SOLO</t>
         </is>
       </c>
       <c r="D198" t="inlineStr">
         <is>
-          <t>Understanding</t>
+          <t>Unistructural</t>
         </is>
       </c>
       <c r="E198" t="inlineStr">
         <is>
-          <t>[('identify', 'Understanding'), ('explain', 'Understanding')]</t>
+          <t>[('identify', 'Unistructural'), ('explain', 'Unistructural')]</t>
         </is>
       </c>
       <c r="F198" t="inlineStr">
         <is>
-          <t>[('describe', 'Understanding'), ('interface', 'Evaluating'), ('lecture', 'Evaluating'), ('characterise', 'Understanding'), ('simulate', 'Applying')]</t>
+          <t>[('describe', 'Unistructural'), ('discern', 'Multistructural'), ('characterise', 'Unistructural'), ('simulate', 'Multistructural'), ('conduct', 'Multistructural')]</t>
         </is>
       </c>
     </row>
@@ -6426,12 +6426,12 @@
       </c>
       <c r="E199" t="inlineStr">
         <is>
-          <t>[('write', 'Applying'), ('interpret', 'Applying')]</t>
+          <t>[('write', 'Applying'), ('interpret', 'Analysing')]</t>
         </is>
       </c>
       <c r="F199" t="inlineStr">
         <is>
-          <t>[('summarise', 'Understanding'), ('derive', 'Applying'), ('order', 'Remembering'), ('compute', 'Applying'), ('conclude', 'Creating')]</t>
+          <t>[('summarise', 'Applying'), ('derive', 'Analysing'), ('order', 'Applying'), ('compute', 'Analysing'), ('conclude', 'Creating')]</t>
         </is>
       </c>
     </row>
@@ -6451,17 +6451,17 @@
       </c>
       <c r="D200" t="inlineStr">
         <is>
-          <t>Applying</t>
+          <t>Analysing</t>
         </is>
       </c>
       <c r="E200" t="inlineStr">
         <is>
-          <t>[('apply', 'Applying')]</t>
+          <t>[('apply', 'Analysing')]</t>
         </is>
       </c>
       <c r="F200" t="inlineStr">
         <is>
-          <t>[('create', 'Creating'), ('summarise', 'Understanding'), ('derive', 'Applying'), ('query', 'Analysing'), ('order', 'Remembering')]</t>
+          <t>[('create', 'Creating'), ('summarise', 'Applying'), ('derive', 'Analysing'), ('query', 'Analysing'), ('order', 'Applying')]</t>
         </is>
       </c>
     </row>
@@ -6491,7 +6491,7 @@
       </c>
       <c r="F201" t="inlineStr">
         <is>
-          <t>[('experiment', 'Analysing'), ('compare', 'Understanding'), ('file', 'Analysing'), ('respond', 'Understanding'), ('document', 'Analysing')]</t>
+          <t>[('experiment', 'Analysing'), ('compare', 'Applying'), ('file', 'Analysing'), ('respond', 'Understanding'), ('document', 'Analysing')]</t>
         </is>
       </c>
     </row>
@@ -6521,7 +6521,7 @@
       </c>
       <c r="F202" t="inlineStr">
         <is>
-          <t>[('extract', 'Analysing'), ('interface', 'Evaluating'), ('file', 'Analysing'), ('example', 'Understanding'), ('trace', 'Remembering')]</t>
+          <t>[('reduce', 'Evaluating'), ('extract', 'Analysing'), ('interface', 'Evaluating'), ('file', 'Analysing'), ('example', 'Understanding')]</t>
         </is>
       </c>
     </row>
@@ -6542,17 +6542,17 @@
       </c>
       <c r="D203" t="inlineStr">
         <is>
-          <t>Understanding</t>
+          <t>Applying</t>
         </is>
       </c>
       <c r="E203" t="inlineStr">
         <is>
-          <t>[('describe', 'Understanding'), ('involve', 'Verb not mapped'), ('include', 'Verb not mapped')]</t>
+          <t>[('describe', 'Applying'), ('involve', 'Verb not mapped'), ('include', 'Verb not mapped')]</t>
         </is>
       </c>
       <c r="F203" t="inlineStr">
         <is>
-          <t>[('factor', 'Understanding'), ('integrate', 'Evaluating'), ('review', 'Remembering'), ('plan', 'Creating'), ('devise', 'Evaluating')]</t>
+          <t>[('factor', 'Understanding'), ('integrate', 'Evaluating'), ('review', 'Analysing'), ('plan', 'Creating'), ('devise', 'Evaluating')]</t>
         </is>
       </c>
     </row>
@@ -6573,17 +6573,17 @@
       </c>
       <c r="D204" t="inlineStr">
         <is>
-          <t>Evaluating</t>
+          <t>Applying</t>
         </is>
       </c>
       <c r="E204" t="inlineStr">
         <is>
-          <t>[('select', 'Evaluating'), ('balance', 'Verb not mapped')]</t>
+          <t>[('select', 'Applying'), ('balance', 'Verb not mapped')]</t>
         </is>
       </c>
       <c r="F204" t="inlineStr">
         <is>
-          <t>[('discuss', 'Understanding'), ('utilise', 'Applying'), ('lecture', 'Evaluating'), ('devise', 'Evaluating'), ('improve', 'Evaluating')]</t>
+          <t>[('discuss', 'Applying'), ('utilise', 'Applying'), ('lecture', 'Evaluating'), ('devise', 'Evaluating'), ('improve', 'Evaluating')]</t>
         </is>
       </c>
     </row>
@@ -6599,22 +6599,22 @@
       </c>
       <c r="C205" t="inlineStr">
         <is>
-          <t>Affective</t>
+          <t>Cognitive</t>
         </is>
       </c>
       <c r="D205" t="inlineStr">
         <is>
-          <t>Characterisation</t>
+          <t>Evaluating</t>
         </is>
       </c>
       <c r="E205" t="inlineStr">
         <is>
-          <t>[('propose', 'Characterisation'), ('improve', 'Verb not mapped'), ('give', 'Receiving')]</t>
+          <t>[('propose', 'Evaluating'), ('improve', 'Evaluating'), ('give', 'Understanding')]</t>
         </is>
       </c>
       <c r="F205" t="inlineStr">
         <is>
-          <t>[('allow', 'Responding'), ('follow', 'Receiving'), ('respond', 'Responding'), ('change', 'Characterisation'), ('select', 'Receiving')]</t>
+          <t>[('provide', 'Applying'), ('respond', 'Understanding'), ('address', 'Evaluating'), ('change', 'Analysing'), ('select', 'Applying')]</t>
         </is>
       </c>
     </row>
@@ -6640,12 +6640,12 @@
       </c>
       <c r="E206" t="inlineStr">
         <is>
-          <t>[('identify', 'Understanding'), ('carry', 'Verb not mapped'), ('conduct', 'Applying'), ('reflect', 'Evaluating')]</t>
+          <t>[('identify', 'Understanding'), ('carry', 'Verb not mapped'), ('conduct', 'Analysing'), ('reflect', 'Evaluating')]</t>
         </is>
       </c>
       <c r="F206" t="inlineStr">
         <is>
-          <t>[('propose', 'Creating'), ('analyse', 'Analysing'), ('explain', 'Understanding'), ('design', 'Creating'), ('construct', 'Creating')]</t>
+          <t>[('propose', 'Evaluating'), ('analyse', 'Analysing'), ('explain', 'Applying'), ('design', 'Creating'), ('construct', 'Evaluating')]</t>
         </is>
       </c>
     </row>
@@ -6665,17 +6665,17 @@
       </c>
       <c r="D207" t="inlineStr">
         <is>
-          <t>Applying</t>
+          <t>Analysing</t>
         </is>
       </c>
       <c r="E207" t="inlineStr">
         <is>
-          <t>[('apply', 'Applying')]</t>
+          <t>[('apply', 'Analysing')]</t>
         </is>
       </c>
       <c r="F207" t="inlineStr">
         <is>
-          <t>[('create', 'Creating'), ('summarise', 'Understanding'), ('derive', 'Applying'), ('query', 'Analysing'), ('order', 'Remembering')]</t>
+          <t>[('create', 'Creating'), ('summarise', 'Applying'), ('derive', 'Analysing'), ('query', 'Analysing'), ('order', 'Applying')]</t>
         </is>
       </c>
     </row>
@@ -6691,22 +6691,22 @@
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>Affective</t>
+          <t>Cognitive</t>
         </is>
       </c>
       <c r="D208" t="inlineStr">
         <is>
-          <t>Organisation</t>
+          <t>Analysing</t>
         </is>
       </c>
       <c r="E208" t="inlineStr">
         <is>
-          <t>[('relate', 'Organisation'), ('establish', 'Organisation')]</t>
+          <t>[('relate', 'Applying'), ('establish', 'Analysing')]</t>
         </is>
       </c>
       <c r="F208" t="inlineStr">
         <is>
-          <t>[('guide', 'Valuing'), ('discuss', 'Responding'), ('collaborate', 'Organisation'), ('generate', 'Organisation'), ('delay', 'Valuing')]</t>
+          <t>[('define', 'Applying'), ('discuss', 'Applying'), ('interface', 'Evaluating'), ('sequence', 'Applying'), ('deliberate', 'Creating')]</t>
         </is>
       </c>
     </row>
@@ -6737,7 +6737,7 @@
       </c>
       <c r="F209" t="inlineStr">
         <is>
-          <t>[('provide', 'Applying'), ('respond', 'Understanding'), ('change', 'Applying'), ('select', 'Evaluating'), ('assess', 'Evaluating')]</t>
+          <t>[('provide', 'Applying'), ('respond', 'Understanding'), ('address', 'Evaluating'), ('change', 'Analysing'), ('select', 'Applying')]</t>
         </is>
       </c>
     </row>
@@ -6753,22 +6753,22 @@
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>SOLO</t>
+          <t>Cognitive</t>
         </is>
       </c>
       <c r="D210" t="inlineStr">
         <is>
-          <t>Relational</t>
+          <t>Applying</t>
         </is>
       </c>
       <c r="E210" t="inlineStr">
         <is>
-          <t>[('perform', 'Relational'), ('relate', 'Relational'), ('provide', 'Verb not mapped')]</t>
+          <t>[('perform', 'Creating'), ('relate', 'Applying'), ('provide', 'Applying')]</t>
         </is>
       </c>
       <c r="F210" t="inlineStr">
         <is>
-          <t>[('order', 'Unistructural'), ('compare', 'Relational'), ('compute', 'Relational'), ('partition', 'Relational'), ('mitigate', 'Extended Abstract')]</t>
+          <t>[('experiment', 'Analysing'), ('order', 'Applying'), ('change', 'Analysing'), ('compare', 'Applying'), ('respond', 'Understanding')]</t>
         </is>
       </c>
     </row>
@@ -6799,7 +6799,7 @@
       </c>
       <c r="F211" t="inlineStr">
         <is>
-          <t>[('justify', 'Valuing'), ('work', 'Valuing'), ('collaborate', 'Organisation'), ('demonstrate', 'Valuing'), ('report', 'Valuing')]</t>
+          <t>[('justify', 'Organisation'), ('work', 'Valuing'), ('collaborate', 'Organisation'), ('demonstrate', 'Responding'), ('report', 'Responding')]</t>
         </is>
       </c>
     </row>
@@ -6819,17 +6819,17 @@
       </c>
       <c r="D212" t="inlineStr">
         <is>
-          <t>Applying</t>
+          <t>Analysing</t>
         </is>
       </c>
       <c r="E212" t="inlineStr">
         <is>
-          <t>[('apply', 'Applying'), ('design', 'Creating'), ('solve', 'Applying')]</t>
+          <t>[('apply', 'Analysing'), ('design', 'Creating'), ('solve', 'Analysing')]</t>
         </is>
       </c>
       <c r="F212" t="inlineStr">
         <is>
-          <t>[('describe', 'Understanding'), ('implement', 'Applying'), ('interface', 'Evaluating'), ('interpret', 'Applying'), ('complete', 'Applying')]</t>
+          <t>[('describe', 'Applying'), ('implement', 'Analysing'), ('interface', 'Evaluating'), ('interpret', 'Analysing'), ('complete', 'Applying')]</t>
         </is>
       </c>
     </row>
@@ -6884,12 +6884,12 @@
       </c>
       <c r="E214" t="inlineStr">
         <is>
-          <t>[('justify', 'Valuing'), ('communicate', 'Responding'), ('write', 'Responding')]</t>
+          <t>[('justify', 'Organisation'), ('communicate', 'Responding'), ('write', 'Responding')]</t>
         </is>
       </c>
       <c r="F214" t="inlineStr">
         <is>
-          <t>[('generate', 'Organisation'), ('prepare', 'Organisation'), ('report', 'Valuing'), ('query', 'Valuing'), ('act', 'Characterisation')]</t>
+          <t>[('generate', 'Organisation'), ('prepare', 'Responding'), ('report', 'Responding'), ('query', 'Valuing'), ('reduce', 'Organisation')]</t>
         </is>
       </c>
     </row>
@@ -6919,7 +6919,7 @@
       </c>
       <c r="F215" t="inlineStr">
         <is>
-          <t>[('conduct', 'Applying'), ('conclude', 'Creating'), ('assign', 'Applying'), ('identify', 'Understanding'), ('compute', 'Applying')]</t>
+          <t>[('conduct', 'Analysing'), ('conclude', 'Creating'), ('assign', 'Applying'), ('identify', 'Understanding'), ('compute', 'Analysing')]</t>
         </is>
       </c>
     </row>
@@ -6939,17 +6939,17 @@
       </c>
       <c r="D216" t="inlineStr">
         <is>
-          <t>Applying</t>
+          <t>Understanding</t>
         </is>
       </c>
       <c r="E216" t="inlineStr">
         <is>
-          <t>[('conduct', 'Applying'), ('deliver', 'Verb not mapped'), ('use', 'Applying'), ('give', 'Understanding')]</t>
+          <t>[('conduct', 'Analysing'), ('deliver', 'Verb not mapped'), ('use', 'Applying'), ('give', 'Understanding')]</t>
         </is>
       </c>
       <c r="F216" t="inlineStr">
         <is>
-          <t>[('provide', 'Applying'), ('respond', 'Understanding'), ('change', 'Applying'), ('select', 'Evaluating'), ('assess', 'Evaluating')]</t>
+          <t>[('provide', 'Applying'), ('respond', 'Understanding'), ('address', 'Evaluating'), ('change', 'Analysing'), ('select', 'Applying')]</t>
         </is>
       </c>
     </row>
@@ -6969,17 +6969,17 @@
       </c>
       <c r="D217" t="inlineStr">
         <is>
-          <t>Applying</t>
+          <t>Analysing</t>
         </is>
       </c>
       <c r="E217" t="inlineStr">
         <is>
-          <t>[('demonstrate', 'Applying')]</t>
+          <t>[('demonstrate', 'Analysing')]</t>
         </is>
       </c>
       <c r="F217" t="inlineStr">
         <is>
-          <t>[('ensure', 'Analysing'), ('detail', 'Understanding'), ('act', 'Applying'), ('monitor', 'Evaluating'), ('adopt', 'Evaluating')]</t>
+          <t>[('engage', 'Creating'), ('ensure', 'Analysing'), ('detail', 'Understanding'), ('act', 'Analysing'), ('monitor', 'Evaluating')]</t>
         </is>
       </c>
     </row>
@@ -7000,17 +7000,17 @@
       </c>
       <c r="D218" t="inlineStr">
         <is>
-          <t>Applying</t>
+          <t>Analysing</t>
         </is>
       </c>
       <c r="E218" t="inlineStr">
         <is>
-          <t>[('appraise', 'Evaluating'), ('apply', 'Applying')]</t>
+          <t>[('appraise', 'Evaluating'), ('apply', 'Analysing')]</t>
         </is>
       </c>
       <c r="F218" t="inlineStr">
         <is>
-          <t>[('create', 'Creating'), ('summarise', 'Understanding'), ('derive', 'Applying'), ('query', 'Analysing'), ('order', 'Remembering')]</t>
+          <t>[('create', 'Creating'), ('summarise', 'Applying'), ('derive', 'Analysing'), ('query', 'Analysing'), ('order', 'Applying')]</t>
         </is>
       </c>
     </row>
@@ -7036,12 +7036,12 @@
       </c>
       <c r="E219" t="inlineStr">
         <is>
-          <t>[('construct', 'Creating'), ('include', 'Verb not mapped'), ('specify', 'Evaluating'), ('require', 'Verb not mapped')]</t>
+          <t>[('construct', 'Evaluating'), ('include', 'Verb not mapped'), ('specify', 'Evaluating'), ('require', 'Verb not mapped')]</t>
         </is>
       </c>
       <c r="F219" t="inlineStr">
         <is>
-          <t>[('complete', 'Applying'), ('lecture', 'Evaluating'), ('specify', 'Evaluating'), ('characterise', 'Understanding'), ('back', 'Applying')]</t>
+          <t>[('complete', 'Applying'), ('lecture', 'Evaluating'), ('specify', 'Evaluating'), ('characterise', 'Applying'), ('back', 'Applying')]</t>
         </is>
       </c>
     </row>
@@ -7067,12 +7067,12 @@
       </c>
       <c r="E220" t="inlineStr">
         <is>
-          <t>[('describe', 'Understanding'), ('use', 'Applying'), ('implement', 'Applying')]</t>
+          <t>[('describe', 'Applying'), ('use', 'Applying'), ('implement', 'Analysing')]</t>
         </is>
       </c>
       <c r="F220" t="inlineStr">
         <is>
-          <t>[('design', 'Creating'), ('debug', 'Evaluating'), ('analyse', 'Analysing'), ('improve', 'Evaluating'), ('construct', 'Creating')]</t>
+          <t>[('function', 'Evaluating'), ('design', 'Creating'), ('debug', 'Evaluating'), ('analyse', 'Analysing'), ('improve', 'Evaluating')]</t>
         </is>
       </c>
     </row>
@@ -7098,12 +7098,12 @@
       </c>
       <c r="E221" t="inlineStr">
         <is>
-          <t>[('design', 'Creating'), ('construct', 'Creating'), ('debug', 'Evaluating'), ('interface', 'Evaluating')]</t>
+          <t>[('design', 'Creating'), ('construct', 'Evaluating'), ('debug', 'Evaluating'), ('interface', 'Evaluating')]</t>
         </is>
       </c>
       <c r="F221" t="inlineStr">
         <is>
-          <t>[('lecture', 'Evaluating'), ('sequence', 'Applying'), ('extract', 'Analysing'), ('change', 'Applying'), ('respond', 'Understanding')]</t>
+          <t>[('lecture', 'Evaluating'), ('sequence', 'Applying'), ('extract', 'Analysing'), ('change', 'Analysing'), ('respond', 'Understanding')]</t>
         </is>
       </c>
     </row>
@@ -7124,17 +7124,17 @@
       </c>
       <c r="D222" t="inlineStr">
         <is>
-          <t>Creating</t>
+          <t>Evaluating</t>
         </is>
       </c>
       <c r="E222" t="inlineStr">
         <is>
-          <t>[('construct', 'Creating'), ('produce', 'Creating')]</t>
+          <t>[('construct', 'Evaluating'), ('produce', 'Creating')]</t>
         </is>
       </c>
       <c r="F222" t="inlineStr">
         <is>
-          <t>[('attribute', 'Evaluating'), ('prepare', 'Applying'), ('experiment', 'Analysing'), ('respond', 'Understanding'), ('change', 'Applying')]</t>
+          <t>[('attribute', 'Evaluating'), ('prepare', 'Analysing'), ('mitigate', 'Creating'), ('experiment', 'Analysing'), ('respond', 'Understanding')]</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Regulatory requirements & small changes
</commit_message>
<xml_diff>
--- a/outputs/all_lo_mappings.xlsx
+++ b/outputs/all_lo_mappings.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,28 +466,27 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Apply knowledge of mathematics, natural science, engineering fundamentals and specialization in Software Engineering to the solution of complex engineering problems;
-</t>
+          <t>describe the underlying theoretical basis of the relational database model and motivations</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>SOLO</t>
+          <t>Cognitive</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Relational</t>
+          <t>Understanding</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>[('apply', 'Relational')]</t>
+          <t>[('describe', 'Understanding'), ('underlie', 'Verb not mapped')]</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>[('organise', 'Relational'), ('explain', 'Relational'), ('define', 'Multistructural'), ('describe', 'Multistructural'), ('determine', 'Multistructural')]</t>
+          <t>[('evaluate', 'Evaluating'), ('model', 'Evaluating'), ('recognise', 'Understanding'), ('research', 'Analysing'), ('describe', 'Understanding')]</t>
         </is>
       </c>
     </row>
@@ -497,8 +496,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Identify, formulate, survey research literature and analyze complex Software engineering problems reaching substantiated conclusions using first principles of mathematics, natural sciences and engineering sciences;
-</t>
+          <t>design a relational database model based on the underlying theoretical basis with the capability of evaluating different options</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -508,17 +506,17 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Analysing</t>
+          <t>Evaluating</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>[('identify', 'Understanding'), ('formulate', 'Creating'), ('survey', 'Analysing'), ('analyze', 'Verb not mapped'), ('reach', 'Verb not mapped'), ('substantiate', 'Evaluating'), ('use', 'Applying')]</t>
+          <t>[('design', 'Creating'), ('base', 'Verb not mapped'), ('underlie', 'Verb not mapped'), ('evaluate', 'Evaluating')]</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>[('programme', 'Evaluating'), ('research', 'Analysing'), ('experiment', 'Analysing'), ('organise', 'Evaluating'), ('develop', 'Creating')]</t>
+          <t>[('recognise', 'Understanding'), ('analyse', 'Analysing'), ('compare', 'Understanding'), ('research', 'Analysing'), ('evaluate', 'Evaluating')]</t>
         </is>
       </c>
     </row>
@@ -528,27 +526,27 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Design solutions for complex Software engineering problems and design systems, components or processes that meet specified needs;</t>
+          <t>implement a database based on a sound database design with constructing queries that meet user requirements</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>SOLO</t>
+          <t>Cognitive</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Extended Abstract</t>
+          <t>Evaluating</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>[('design', 'Extended Abstract'), ('design', 'Extended Abstract'), ('meet', 'Verb not mapped'), ('specify', 'Verb not mapped')]</t>
+          <t>[('implement', 'Applying'), ('base', 'Verb not mapped'), ('construct', 'Creating'), ('meet', 'Remembering')]</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>[('plan', 'Extended Abstract'), ('implement', 'Relational'), ('review', 'Extended Abstract'), ('evaluate', 'Extended Abstract'), ('process', 'Multistructural')]</t>
+          <t>[('evaluate', 'Evaluating'), ('produce', 'Creating'), ('design', 'Creating'), ('comprehend', 'Understanding'), ('support', 'Evaluating')]</t>
         </is>
       </c>
     </row>
@@ -558,7 +556,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Conduct investigations of complex Software engineering problems using research-based knowledge and research methods including design of experiments, analysis and interpretation of data, and synthesis of information to provide valid conclusions;</t>
+          <t>contrast the differences between non-relational database models and the relational database model.</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -568,17 +566,17 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Applying</t>
+          <t>Analysing</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>[('conduct', 'Applying'), ('use', 'Applying'), ('base', 'Verb not mapped'), ('include', 'Verb not mapped'), ('provide', 'Applying')]</t>
+          <t>[('contrast', 'Analysing')]</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>[('explain', 'Understanding'), ('research', 'Analysing'), ('determine', 'Analysing'), ('demonstrate', 'Applying'), ('substantiate', 'Evaluating')]</t>
+          <t>[('evaluate', 'Evaluating'), ('analyse', 'Analysing'), ('compare', 'Understanding'), ('recognise', 'Understanding'), ('abstract', 'Evaluating')]</t>
         </is>
       </c>
     </row>
@@ -588,27 +586,27 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Create, select and apply appropriate techniques, resources, and modern engineering and IT tools, including prediction and modelling, to complex Software engineering problems, with an understanding of the limitations;</t>
+          <t>develop programming structures within a database backend.</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Affective</t>
+          <t>Cognitive</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Receiving</t>
+          <t>Creating</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>[('create', 'Verb not mapped'), ('select', 'Receiving'), ('apply', 'Verb not mapped'), ('include', 'Verb not mapped')]</t>
+          <t>[('develop', 'Creating')]</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>[('identify', 'Receiving'), ('support', 'Valuing'), ('manage', 'Organisation'), ('organise', 'Organisation'), ('justify', 'Valuing')]</t>
+          <t>[('design', 'Creating'), ('use', 'Applying'), ('debug', 'Evaluating'), ('document', 'Analysing'), ('analyse', 'Analysing')]</t>
         </is>
       </c>
     </row>
@@ -618,7 +616,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Apply reasoning informed by contextual knowledge to assess societal, health, safety, legal and cultural issues and the consequent responsibilities relevant to professional engineering practice and solutions to complex Software engineering problems;</t>
+          <t>discuss requirements of a smart system from component to integrated perspective.</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -628,17 +626,17 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Applying</t>
+          <t>Understanding</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>[('apply', 'Applying'), ('inform', 'Verb not mapped'), ('assess', 'Evaluating')]</t>
+          <t>[('discuss', 'Understanding'), ('integrate', 'Evaluating')]</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>[('assess', 'Evaluating'), ('support', 'Evaluating'), ('comprehend', 'Understanding'), ('explain', 'Understanding'), ('apply', 'Applying')]</t>
+          <t>[('research', 'Analysing'), ('give', 'Understanding'), ('substantiate', 'Evaluating'), ('translate', 'Understanding'), ('evaluate', 'Evaluating')]</t>
         </is>
       </c>
     </row>
@@ -648,27 +646,27 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Understand and evaluate the sustainability and impact of professional engineering work in the solution of complex Software engineering problems in environmental contexts;</t>
+          <t>define programs using python, discern problem-solving strategies in decomposing problems using algorithms and describe software engineering processes.</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Cognitive</t>
+          <t>SOLO</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Analysing</t>
+          <t>Multistructural</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>[('understand', 'Verb not mapped'), ('evaluate', 'Evaluating')]</t>
+          <t>[('define', 'Multistructural'), ('use', 'Relational'), ('discern', 'Multistructural'), ('solve', 'Multistructural'), ('decompose', 'Verb not mapped'), ('use', 'Relational'), ('describe', 'Multistructural')]</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>[('recognise', 'Understanding'), ('analyse', 'Analysing'), ('compare', 'Understanding'), ('research', 'Analysing'), ('construct', 'Creating')]</t>
+          <t>[('write', 'Unistructural'), ('analyse', 'Relational'), ('identify', 'Unistructural'), ('recognise', 'Unistructural'), ('discern', 'Multistructural')]</t>
         </is>
       </c>
     </row>
@@ -678,7 +676,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Apply ethical principles and commit to professional ethics and responsibilities and norms of engineering practice;</t>
+          <t>select fundamental circuit analysis techniques to solve problems in circuits that contain common electrical and electronic components.</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -688,17 +686,17 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Relational</t>
+          <t>Multistructural</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>[('apply', 'Relational'), ('commit', 'Verb not mapped')]</t>
+          <t>[('select', 'Multistructural'), ('solve', 'Multistructural'), ('contain', 'Verb not mapped')]</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>[('apply', 'Relational'), ('define', 'Multistructural'), ('discern', 'Multistructural'), ('explain', 'Relational'), ('engage', 'Extended Abstract')]</t>
+          <t>[('use', 'Relational'), ('discern', 'Multistructural'), ('analyse', 'Relational'), ('define', 'Multistructural'), ('explain', 'Relational')]</t>
         </is>
       </c>
     </row>
@@ -708,27 +706,27 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Communicate effectively on complex Software engineering activities with the engineering community and with society at large, such as being able to comprehend and write effective reports and design documentation, make effective presentations, and give and receive clear instructions;</t>
+          <t>propose a design solution in response to a given scenario through requirements and functional analysis, evaluate that solution from an integrated system perspective.</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Affective</t>
+          <t>Cognitive</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Valuing</t>
+          <t>Analysing</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>[('communicate', 'Responding'), ('comprehend', 'Verb not mapped'), ('write', 'Responding'), ('design', 'Organisation'), ('make', 'Verb not mapped'), ('give', 'Receiving'), ('receive', 'Receiving')]</t>
+          <t>[('propose', 'Creating'), ('give', 'Understanding'), ('evaluate', 'Evaluating')]</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>[('form', 'Valuing'), ('adopt', 'Valuing'), ('describe', 'Receiving'), ('write', 'Responding'), ('justify', 'Valuing')]</t>
+          <t>[('recognise', 'Understanding'), ('analyse', 'Analysing'), ('compare', 'Understanding'), ('research', 'Analysing'), ('construct', 'Creating')]</t>
         </is>
       </c>
     </row>
@@ -738,28 +736,27 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t xml:space="preserve">Function effectively as an individual, and as a member or leader in diverse teams and in multi-disciplinary settings;
-</t>
+          <t>identify appropriate engineering tools and techniques to develop and validate a solution.</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Affective</t>
+          <t>Cognitive</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Characterisation</t>
+          <t>Understanding</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>[('function', 'Characterisation')]</t>
+          <t>[('identify', 'Understanding'), ('develop', 'Creating'), ('validate', 'Evaluating')]</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>[('communicate', 'Responding'), ('evaluate', 'Valuing'), ('identify', 'Receiving'), ('recognise', 'Receiving'), ('explain', 'Valuing')]</t>
+          <t>[('identify', 'Understanding'), ('construct', 'Creating'), ('define', 'Remembering'), ('use', 'Applying'), ('support', 'Evaluating')]</t>
         </is>
       </c>
     </row>
@@ -769,27 +766,27 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Recognize the need for, and have the preparation and ability to engage in independent and life-long learning in the broadest context of technological change;</t>
+          <t>identify the ethical considerations of data collection and analysis in engineering designs that may impact the suitability of solutions.</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>SOLO</t>
+          <t>Cognitive</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Extended Abstract</t>
+          <t>Understanding</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>[('recognize', 'Verb not mapped'), ('have', 'Verb not mapped'), ('engage', 'Extended Abstract')]</t>
+          <t>[('identify', 'Understanding'), ('impact', 'Verb not mapped')]</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>[('demonstrate', 'Extended Abstract'), ('recognise', 'Unistructural'), ('determine', 'Multistructural'), ('identify', 'Unistructural'), ('review', 'Extended Abstract')]</t>
+          <t>[('propose', 'Creating'), ('substantiate', 'Evaluating'), ('write', 'Applying'), ('evaluate', 'Evaluating'), ('research', 'Analysing')]</t>
         </is>
       </c>
     </row>
@@ -799,27 +796,2280 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Demonstrate knowledge and understanding of engineering management principles and economic decision-making and apply these to manage projects;</t>
+          <t>describe project progress and outputs to stakeholders in review meetings, demonstrations and documentation.</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
+          <t>Cognitive</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Understanding</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>[('describe', 'Understanding')]</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>[('write', 'Applying'), ('analyse', 'Analysing'), ('identify', 'Understanding'), ('research', 'Analysing'), ('recognise', 'Understanding')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>identify roles and responsibilities within a team and reflect on self and team behaviours that contribute to the successful conduct of a project.</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Cognitive</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Understanding</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>[('identify', 'Understanding'), ('reflect', 'Evaluating'), ('contribute', 'Verb not mapped')]</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>[('reflect', 'Evaluating'), ('conduct', 'Applying'), ('describe', 'Understanding'), ('identify', 'Understanding'), ('ensure', 'Analysing')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>discern fundamental chemical, materials, mechanical and environmental engineering knowledge, principles and concepts to propose solutions to a humanitarian engineering problem.</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
           <t>SOLO</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Multistructural</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>[('discern', 'Multistructural'), ('propose', 'Multistructural')]</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>[('analyse', 'Relational'), ('design', 'Extended Abstract'), ('write', 'Unistructural'), ('select', 'Multistructural'), ('justify', 'Extended Abstract')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>identify design requirements from a provided brief and analyse potential solutions using first principles of mathematics and natural and engineering sciences.</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Cognitive</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Understanding</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>[('identify', 'Understanding'), ('provide', 'Applying'), ('analyse', 'Analysing'), ('use', 'Applying')]</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>[('programme', 'Evaluating'), ('research', 'Analysing'), ('experiment', 'Analysing'), ('organise', 'Evaluating'), ('develop', 'Creating')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>identify societal, health, safety, legal and cultural issues relevant to your project including the indigenous context, and your consequent responsibilities as an engineer.</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Cognitive</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Understanding</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>[('identify', 'Understanding'), ('include', 'Verb not mapped')]</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>[('identify', 'Understanding'), ('support', 'Evaluating'), ('project', 'Applying'), ('utilise', 'Applying'), ('manage', 'Analysing')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>determine appropriate principles of sustainable design and development, including embodied energy, renewable materials, availability, costs, etc, of a proposed solution using a systems approach to design.</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Cognitive</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Analysing</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>[('determine', 'Analysing'), ('include', 'Verb not mapped'), ('propose', 'Creating'), ('use', 'Applying')]</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>[('programme', 'Evaluating'), ('research', 'Analysing'), ('experiment', 'Analysing'), ('organise', 'Evaluating'), ('develop', 'Creating')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>discern the ethical considerations of working with diverse communities and stakeholders, and demonstrate your commitment to the engineers australia code of ethics and/or the board of engineers malaysia code of professional conduct, and established norms of professional conduct throughout your project.</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>SOLO</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Multistructural</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>[('discern', 'Multistructural'), ('work', 'Verb not mapped'), ('demonstrate', 'Extended Abstract'), ('establish', 'Verb not mapped')]</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>[('organise', 'Relational'), ('report', 'Multistructural'), ('demonstrate', 'Extended Abstract'), ('define', 'Multistructural'), ('discern', 'Multistructural')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>describe project progress and outputs to stakeholders verbally through pitches, in writing through professional engineering documentation, and graphically through drawings and visualisations.</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Cognitive</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Understanding</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>[('describe', 'Understanding')]</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>[('write', 'Applying'), ('analyse', 'Analysing'), ('identify', 'Understanding'), ('research', 'Analysing'), ('recognise', 'Understanding')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>describe the principles of team norms, collaboration and dynamics, define your professional practice goals and discern the practices that lead to successful teamwork in a multicultural context.</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>SOLO</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Multistructural</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>[('describe', 'Multistructural'), ('define', 'Multistructural'), ('discern', 'Multistructural'), ('lead', 'Verb not mapped')]</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>[('engage', 'Extended Abstract'), ('define', 'Multistructural'), ('determine', 'Multistructural'), ('review', 'Extended Abstract'), ('demonstrate', 'Extended Abstract')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>design and implement a software system of a quality acceptable to an external client</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Cognitive</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Applying</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>[('design', 'Creating'), ('implement', 'Applying')]</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>[('research', 'Analysing'), ('analyse', 'Analysing'), ('devise', 'Evaluating'), ('support', 'Evaluating'), ('ensure', 'Analysing')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">select and use appropriate tools, techniques and strategies to manage project resources, 
+including time and personnel </t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Affective</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Receiving</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>[('select', 'Receiving'), ('use', 'Receiving'), ('manage', 'Organisation'), ('include', 'Verb not mapped')]</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>[('identify', 'Receiving'), ('support', 'Valuing'), ('manage', 'Organisation'), ('organise', 'Organisation'), ('justify', 'Valuing')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>identify potential sources of risk, including ethical risk, and devise and adopt appropriate strategies to monitor and mitigate these risks</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Cognitive</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Evaluating</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>[('identify', 'Understanding'), ('include', 'Verb not mapped'), ('devise', 'Evaluating'), ('adopt', 'Evaluating'), ('monitor', 'Evaluating'), ('mitigate', 'Verb not mapped')]</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>[('devise', 'Evaluating'), ('determine', 'Analysing'), ('give', 'Understanding'), ('measure', 'Evaluating'), ('monitor', 'Evaluating')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>choose and follow a software development methodology that is appropriate to the team, project and client, and justify this methodology</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Affective</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Receiving</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>[('choose', 'Receiving'), ('follow', 'Receiving'), ('justify', 'Valuing')]</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>[('write', 'Responding'), ('form', 'Valuing'), ('report', 'Valuing'), ('give', 'Receiving'), ('support', 'Valuing')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>elicit requirements from client representatives and ensure that these are communicated to team members and other stakeholders in an appropriate form</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Cognitive</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Analysing</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>[('elicit', 'Verb not mapped'), ('ensure', 'Analysing'), ('communicate', 'Verb not mapped')]</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>[('demonstrate', 'Applying'), ('research', 'Analysing'), ('recognise', 'Understanding'), ('measure', 'Evaluating'), ('relate', 'Remembering')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">produce internal documentation of a sufficient quality to support project development 
+activities (including specification, analysis, design, testing); </t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Cognitive</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Understanding</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>[('produce', 'Creating'), ('support', 'Evaluating'), ('include', 'Verb not mapped')]</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>[('identify', 'Understanding'), ('support', 'Evaluating'), ('project', 'Applying'), ('utilise', 'Applying'), ('manage', 'Analysing')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>communicate effectively with other project stakeholders, including clients, end users, and supervisors</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Cognitive</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Applying</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>[('communicate', 'Verb not mapped'), ('include', 'Verb not mapped')]</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>[('identify', 'Understanding'), ('support', 'Evaluating'), ('project', 'Applying'), ('utilise', 'Applying'), ('manage', 'Analysing')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">verify systematically that internal and external project deliverables meet agreed quality 
+standards </t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Cognitive</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Remembering</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>[('verify', 'Creating'), ('meet', 'Remembering'), ('agree', 'Verb not mapped')]</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>[('evaluate', 'Evaluating'), ('contrast', 'Analysing'), ('meet', 'Remembering'), ('research', 'Analysing'), ('diagram', 'Analysing')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>produce external documentation of a sufficient quality to meet the needs of clients, end users, and client-site technical staff.</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Cognitive</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Remembering</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>[('produce', 'Creating'), ('meet', 'Remembering')]</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>[('evaluate', 'Evaluating'), ('produce', 'Creating'), ('meet', 'Remembering'), ('design', 'Creating'), ('comprehend', 'Understanding')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>analyse general problem solving strategies and algorithmic paradigms</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Cognitive</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Evaluating</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>[('analyse', 'Analysing')]</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>[('evaluate', 'Evaluating'), ('measure', 'Evaluating'), ('research', 'Analysing'), ('describe', 'Understanding'), ('determine', 'Analysing')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>prove correctness of programs, analyse their space and time complexities.</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Cognitive</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Evaluating</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>[('prove', 'Evaluating'), ('analyse', 'Analysing')]</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>[('evaluate', 'Evaluating'), ('measure', 'Evaluating'), ('research', 'Analysing'), ('describe', 'Understanding'), ('determine', 'Analysing')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>compare and contrast various abstract data types and use them appropriately.</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>SOLO</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
         <is>
           <t>Relational</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>[('demonstrate', 'Extended Abstract'), ('apply', 'Relational'), ('manage', 'Relational')]</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>[('organise', 'Relational'), ('plan', 'Extended Abstract'), ('identify', 'Unistructural'), ('describe', 'Multistructural'), ('manage', 'Relational')]</t>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>[('compare', 'Relational'), ('contrast', 'Relational'), ('use', 'Relational')]</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>[('organise', 'Relational'), ('develop', 'Extended Abstract'), ('apply', 'Relational'), ('discern', 'Multistructural'), ('propose', 'Multistructural')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>develop and implement algorithms to solve computational problems.</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Cognitive</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Applying</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>[('develop', 'Creating'), ('implement', 'Applying'), ('solve', 'Applying')]</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>[('network', 'Evaluating'), ('describe', 'Understanding'), ('research', 'Analysing'), ('solve', 'Applying'), ('implement', 'Applying')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>determine reactions and internal member forces in simple truss and beam systems and carry out limit state design to select appropriately sized members.</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Cognitive</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Analysing</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>[('determine', 'Analysing'), ('carry', 'Verb not mapped'), ('select', 'Evaluating')]</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>[('identify', 'Understanding'), ('state', 'Remembering'), ('measure', 'Evaluating'), ('propose', 'Creating'), ('document', 'Analysing')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>determine the strength of structural materials to inform engineering designs with considerations to performance. cost, sustainability and societal impact.</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Cognitive</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Analysing</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>[('determine', 'Analysing'), ('inform', 'Verb not mapped')]</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>[('allocate', 'Applying'), ('utilise', 'Applying'), ('analyse', 'Analysing'), ('write', 'Applying'), ('determine', 'Analysing')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>determine the steady-state performance of simple systems involving levers, gears, springs and pulleys using appropriate engineering problem-solving methodologies.</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Cognitive</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Analysing</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>[('determine', 'Analysing'), ('involve', 'Verb not mapped'), ('use', 'Applying'), ('solve', 'Applying')]</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>[('network', 'Evaluating'), ('describe', 'Understanding'), ('research', 'Analysing'), ('implement', 'Applying'), ('evaluate', 'Evaluating')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>analyse concept designs that solve engineering problems and justify finalised design with considerations of key variables, assumptions, and system boundaries.</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>SOLO</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Multistructural</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>[('analyse', 'Relational'), ('solve', 'Multistructural'), ('justify', 'Extended Abstract'), ('finalise', 'Verb not mapped')]</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>[('analyse', 'Relational'), ('review', 'Extended Abstract'), ('evaluate', 'Extended Abstract'), ('process', 'Multistructural'), ('list', 'Multistructural')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>propose concept designs and develop a final design which balances competing requirements.</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Cognitive</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Creating</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>[('propose', 'Creating'), ('develop', 'Creating'), ('balance', 'Verb not mapped'), ('compete', 'Verb not mapped')]</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>[('research', 'Analysing'), ('analyse', 'Analysing'), ('construct', 'Creating'), ('ensure', 'Analysing'), ('comprehend', 'Understanding')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>identify appropriate engineering tools and techniques to develop, validate and convey designs and solutions.</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Cognitive</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Understanding</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>[('identify', 'Understanding'), ('develop', 'Creating'), ('validate', 'Evaluating'), ('convey', 'Verb not mapped')]</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>[('use', 'Applying'), ('provide', 'Applying'), ('propose', 'Creating'), ('explain', 'Understanding'), ('analyse', 'Analysing')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>identify roles and responsibilities within a team and reflect on self and team behaviours that contribute to the successful conduct of a project.</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Cognitive</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Understanding</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>[('identify', 'Understanding'), ('reflect', 'Evaluating'), ('contribute', 'Verb not mapped')]</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>[('reflect', 'Evaluating'), ('conduct', 'Applying'), ('describe', 'Understanding'), ('identify', 'Understanding'), ('ensure', 'Analysing')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>apply suitable mathematical techniques to solve problems involving linear algebra, multi-variable calculus and ordinary differential equations.</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>SOLO</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Relational</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>[('apply', 'Relational'), ('solve', 'Multistructural'), ('involve', 'Verb not mapped')]</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>[('identify', 'Unistructural'), ('implement', 'Relational'), ('review', 'Extended Abstract'), ('analyse', 'Relational'), ('determine', 'Multistructural')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>design object-oriented solutions for small to medium-size systems using standard software engineering notations such as uml diagrams. (c5)</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Cognitive</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Analysing</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>[('design', 'Creating'), ('orient', 'Verb not mapped'), ('use', 'Applying')]</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>[('programme', 'Evaluating'), ('research', 'Analysing'), ('experiment', 'Analysing'), ('organise', 'Evaluating'), ('develop', 'Creating')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>develop object-oriented designs in an object-oriented programming language such as java, using object-oriented programming constructs such as classes, inheritance, abstract classes, and generics. (c5).</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Cognitive</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Analysing</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>[('develop', 'Creating'), ('orient', 'Verb not mapped'), ('orient', 'Verb not mapped'), ('use', 'Applying'), ('orient', 'Verb not mapped')]</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>[('programme', 'Evaluating'), ('research', 'Analysing'), ('experiment', 'Analysing'), ('organise', 'Evaluating'), ('develop', 'Creating')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>apply available language tools, such as debuggers and profilers, and good programming practice to debug their implementations systematically and efficiently. (c3)</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Cognitive</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Evaluating</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>[('apply', 'Applying'), ('debug', 'Evaluating')]</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>[('review', 'Remembering'), ('evaluate', 'Evaluating'), ('give', 'Understanding'), ('support', 'Evaluating'), ('recognise', 'Understanding')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>evaluate the quality of object-oriented software designs both in terms of meeting user requirements and in terms of good design principles, using appropriate domain vocabulary. (c6)</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Cognitive</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Analysing</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>[('evaluate', 'Evaluating'), ('orient', 'Verb not mapped'), ('meet', 'Remembering'), ('use', 'Applying')]</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>[('programme', 'Evaluating'), ('research', 'Analysing'), ('experiment', 'Analysing'), ('organise', 'Evaluating'), ('develop', 'Creating')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>apply knowledge of networking fundamentals, and advanced networking knowledge appropriate to solve complex networking problems and network design problems (c3)</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Cognitive</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Applying</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>[('apply', 'Applying'), ('solve', 'Applying')]</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>[('network', 'Evaluating'), ('describe', 'Understanding'), ('research', 'Analysing'), ('implement', 'Applying'), ('evaluate', 'Evaluating')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>analyse the computer network problems from different layers of internet model using appropriate mechanism (c4)</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Cognitive</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Analysing</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>[('analyse', 'Analysing'), ('use', 'Applying')]</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>[('programme', 'Evaluating'), ('research', 'Analysing'), ('experiment', 'Analysing'), ('organise', 'Evaluating'), ('develop', 'Creating')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>design wired and/or wireless networks that can optimise network performance subject to various resource constraints (c6)</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Cognitive</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Analysing</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>[('design', 'Creating'), ('optimise', 'Analysing')]</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>[('identify', 'Understanding'), ('determine', 'Analysing'), ('allocate', 'Applying'), ('organise', 'Evaluating'), ('network', 'Evaluating')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>select and use appropriate techniques and software tools to investigate complex computer networking related practical problems</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Psychomotor</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Perception</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>[('select', 'Perception'), ('use', 'Verb not mapped'), ('investigate', 'Verb not mapped'), ('relate', 'Perception')]</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>[('state', 'Set'), ('identify', 'Perception'), ('describe', 'Perception'), ('recognise', 'Perception'), ('explain', 'Set')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>analyse simple logic circuits;</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Cognitive</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Evaluating</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>[('analyse', 'Analysing')]</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>[('evaluate', 'Evaluating'), ('measure', 'Evaluating'), ('research', 'Analysing'), ('describe', 'Understanding'), ('determine', 'Analysing')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>explain and analyse key processor components;</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Cognitive</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Evaluating</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>[('explain', 'Understanding'), ('analyse', 'Analysing')]</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>[('evaluate', 'Evaluating'), ('measure', 'Evaluating'), ('research', 'Analysing'), ('describe', 'Understanding'), ('determine', 'Analysing')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>explain and analyse computer organisation;</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Cognitive</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Evaluating</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>[('explain', 'Understanding'), ('analyse', 'Analysing')]</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>[('evaluate', 'Evaluating'), ('measure', 'Evaluating'), ('research', 'Analysing'), ('describe', 'Understanding'), ('determine', 'Analysing')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>write and debug simple assembly language programs;</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Affective</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Valuing</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>[('write', 'Responding'), ('debug', 'Verb not mapped')]</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>[('evaluate', 'Valuing'), ('give', 'Receiving'), ('support', 'Valuing'), ('recognise', 'Receiving'), ('identify', 'Receiving')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>use simulator programs to model computer system components.</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Cognitive</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Evaluating</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>[('use', 'Applying'), ('model', 'Evaluating')]</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>[('recognise', 'Understanding'), ('evaluate', 'Evaluating'), ('describe', 'Understanding'), ('research', 'Analysing'), ('diagram', 'Analysing')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>apply engineering fundamentals to design a mechatronics system.</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Affective</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Organisation</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>[('apply', 'Verb not mapped'), ('design', 'Organisation')]</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>[('develop', 'Organisation'), ('propose', 'Characterisation'), ('meet', 'Receiving'), ('evaluate', 'Valuing'), ('support', 'Valuing')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>design a complex mechatronics system that meets design requirements.</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>SOLO</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Extended Abstract</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>[('design', 'Extended Abstract'), ('meet', 'Verb not mapped')]</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>[('evaluate', 'Extended Abstract'), ('design', 'Extended Abstract'), ('implement', 'Relational'), ('determine', 'Multistructural'), ('identify', 'Unistructural')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>propose an appropriate design methodology to achieve design requirements.</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>SOLO</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Multistructural</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>[('propose', 'Multistructural'), ('achieve', 'Verb not mapped')]</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>[('determine', 'Multistructural'), ('justify', 'Extended Abstract'), ('describe', 'Multistructural'), ('select', 'Multistructural'), ('propose', 'Multistructural')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>identify and use appropriate techniques, resources and modern engineering tools to achieve the design requirements.</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Cognitive</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Understanding</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>[('identify', 'Understanding'), ('use', 'Applying'), ('achieve', 'Verb not mapped')]</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>[('determine', 'Analysing'), ('give', 'Understanding'), ('project', 'Applying'), ('research', 'Analysing'), ('justify', 'Creating')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>justify technical details of a mechatronics solution(s) in written and oral forms.</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Affective</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Valuing</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>[('justify', 'Valuing'), ('write', 'Responding')]</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>[('justify', 'Valuing'), ('write', 'Responding'), ('report', 'Valuing'), ('describe', 'Receiving'), ('form', 'Valuing')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>demonstrate the ability to work effectively as a member or leader in a diverse team.</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Affective</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Valuing</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>[('demonstrate', 'Valuing'), ('work', 'Valuing')]</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>[('communicate', 'Responding'), ('demonstrate', 'Valuing'), ('work', 'Valuing'), ('establish', 'Organisation'), ('explain', 'Valuing')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>manage a project and drive it to successful completion.</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Affective</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Organisation</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>[('manage', 'Organisation'), ('drive', 'Verb not mapped')]</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>[('identify', 'Receiving'), ('organise', 'Organisation'), ('give', 'Receiving'), ('propose', 'Characterisation'), ('recognise', 'Receiving')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>demonstrate an understanding of the motivation for engineers to carry out mechatronics design.</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Cognitive</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Analysing</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>[('demonstrate', 'Applying'), ('carry', 'Verb not mapped')]</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>[('comprehend', 'Understanding'), ('research', 'Analysing'), ('document', 'Analysing'), ('construct', 'Creating'), ('analyse', 'Analysing')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>carry out investigations to identify suitable software quality and quality assurance measures, including human review and inspection of code and non-code artifacts, as well as execution-based testing</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Cognitive</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Understanding</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>[('carry', 'Verb not mapped'), ('identify', 'Understanding'), ('include', 'Verb not mapped'), ('base', 'Verb not mapped')]</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>[('model', 'Evaluating'), ('plan', 'Creating'), ('recognise', 'Understanding'), ('identify', 'Understanding'), ('query', 'Analysing')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>apply specific and appropriate quality goals for a moderately-sized software development project, select an appropriate quality assurance strategy to give confidence that these quality goals can be achieved, and document this strategy appropriately in the context of a software process model</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Cognitive</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>Understanding</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>[('apply', 'Applying'), ('select', 'Evaluating'), ('give', 'Understanding'), ('achieve', 'Verb not mapped'), ('document', 'Analysing')]</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>[('state', 'Remembering'), ('give', 'Understanding'), ('analyse', 'Analysing'), ('allocate', 'Applying'), ('evaluate', 'Evaluating')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>perform systematic, automated unit testing on source code modules, using both specification-based and code-based approaches, utilising automated testing frameworks, including faking and mocking tools</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Cognitive</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>Applying</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>[('perform', 'Creating'), ('use', 'Applying'), ('base', 'Verb not mapped'), ('base', 'Verb not mapped'), ('utilise', 'Applying'), ('automate', 'Verb not mapped'), ('include', 'Verb not mapped')]</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>[('identify', 'Understanding'), ('support', 'Evaluating'), ('project', 'Applying'), ('utilise', 'Applying'), ('manage', 'Analysing')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>evaluate different strategies for solving and translating problem statements into algorithms and implement them in a high level programming language.</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>SOLO</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>Relational</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>[('evaluate', 'Extended Abstract'), ('solve', 'Multistructural'), ('translate', 'Relational'), ('implement', 'Relational')]</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>[('analyse', 'Relational'), ('construct', 'Relational'), ('organise', 'Relational'), ('identify', 'Unistructural'), ('determine', 'Multistructural')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>summarise, compare, design, and theoretically and experimentally evaluate different algorithms and implementations of basic abstract data types such as stacks, queues, lists, trees, priority queues, heaps and hash tables.</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>SOLO</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>Relational</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>[('summarise', 'Relational'), ('compare', 'Relational'), ('design', 'Extended Abstract'), ('evaluate', 'Extended Abstract')]</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>[('recognise', 'Unistructural'), ('analyse', 'Relational'), ('compare', 'Relational'), ('construct', 'Relational'), ('contrast', 'Relational')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>analyse algorithms by determining their best/worst case big o time complexity and recognize their limitations, both theoretical and practical.</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Cognitive</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>Analysing</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>[('analyse', 'Analysing'), ('determine', 'Analysing'), ('recognize', 'Verb not mapped')]</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>[('support', 'Evaluating'), ('give', 'Understanding'), ('review', 'Remembering'), ('justify', 'Creating'), ('substantiate', 'Evaluating')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>deconstruct simple high-level code into assembly code such as mips r2000</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Cognitive</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>Analysing</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>[('deconstruct', 'Analysing')]</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>[('code', 'Evaluating'), ('determine', 'Analysing'), ('review', 'Remembering'), ('justify', 'Creating'), ('identify', 'Understanding')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>model and design flexible software at the architectural level using various tools and techniques;</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Cognitive</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>Evaluating</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>[('model', 'Evaluating'), ('design', 'Creating'), ('use', 'Applying')]</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>[('programme', 'Evaluating'), ('research', 'Analysing'), ('experiment', 'Analysing'), ('organise', 'Evaluating'), ('develop', 'Creating')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>analyse and design software systems taking into consideration various quality attributes and requirements;</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Cognitive</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>Evaluating</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>[('analyse', 'Analysing'), ('design', 'Creating'), ('take', 'Verb not mapped')]</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>[('analyse', 'Analysing'), ('state', 'Remembering'), ('give', 'Understanding'), ('review', 'Remembering'), ('determine', 'Analysing')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>analyse, identify, and take requirements for simple systems and develop software architectures and designs at a high level</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Cognitive</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>Understanding</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>[('analyse', 'Analysing'), ('identify', 'Understanding'), ('take', 'Verb not mapped'), ('develop', 'Creating')]</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>[('design', 'Creating'), ('use', 'Applying'), ('debug', 'Evaluating'), ('document', 'Analysing'), ('analyse', 'Analysing')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="n">
+        <v>72</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>identify and use configuration management tools effectively</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Affective</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>Receiving</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>[('identify', 'Receiving'), ('use', 'Receiving')]</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>[('organise', 'Organisation'), ('develop', 'Organisation'), ('communicate', 'Responding'), ('propose', 'Characterisation'), ('establish', 'Organisation')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="n">
+        <v>73</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>apply a variety of design patterns, frameworks and architectures in designing software;</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Affective</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>Organisation</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>[('apply', 'Verb not mapped'), ('design', 'Organisation')]</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>[('develop', 'Organisation'), ('propose', 'Characterisation'), ('meet', 'Receiving'), ('evaluate', 'Valuing'), ('support', 'Valuing')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>identify, locate and use off-the-shelf components in the construction of software.</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Affective</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>Receiving</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>[('identify', 'Receiving'), ('locate', 'Receiving'), ('use', 'Receiving')]</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>[('organise', 'Organisation'), ('develop', 'Organisation'), ('communicate', 'Responding'), ('propose', 'Characterisation'), ('establish', 'Organisation')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>describe industry-standard team-based project management methodologies and apply them across a multi-functional team to achieve optimal project progress</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Affective</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>Receiving</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>[('describe', 'Receiving'), ('base', 'Verb not mapped'), ('apply', 'Verb not mapped'), ('achieve', 'Verb not mapped')]</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>[('give', 'Receiving'), ('justify', 'Valuing'), ('describe', 'Receiving'), ('select', 'Receiving'), ('receive', 'Receiving')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>plan and manage the full range of activities in a software engineering project in accordance with the development methodology</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Affective</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>Organisation</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>[('plan', 'Organisation'), ('manage', 'Organisation')]</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>[('organise', 'Organisation'), ('plan', 'Organisation'), ('manage', 'Organisation'), ('identify', 'Receiving'), ('describe', 'Receiving')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>apply soft skills when engaging stakeholders in a consistent and professional manner to determine functional and non-functional requirements</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>SOLO</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>Extended Abstract</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>[('apply', 'Relational'), ('engage', 'Extended Abstract'), ('determine', 'Multistructural')]</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>[('review', 'Extended Abstract'), ('justify', 'Extended Abstract'), ('engage', 'Extended Abstract'), ('determine', 'Multistructural'), ('analyse', 'Relational')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>identify aspects of quality that are important in the context of the project, and devise and implement strategies for ensuring quality goals are met;</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Cognitive</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>Evaluating</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>[('identify', 'Understanding'), ('devise', 'Evaluating'), ('implement', 'Applying'), ('ensure', 'Analysing'), ('meet', 'Remembering')]</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>[('evaluate', 'Evaluating'), ('produce', 'Creating'), ('design', 'Creating'), ('comprehend', 'Understanding'), ('support', 'Evaluating')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>compare and analyse appropriate industry-standard technologies to determine the optimal combination of software required to support project development</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Cognitive</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>Analysing</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>[('compare', 'Understanding'), ('analyse', 'Analysing'), ('determine', 'Analysing'), ('require', 'Verb not mapped'), ('support', 'Evaluating')]</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>[('make', 'Creating'), ('determine', 'Analysing'), ('support', 'Evaluating'), ('research', 'Analysing'), ('identify', 'Understanding')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>analyse and deliberate professional issues occurring within the development and deployment of software applications, and identify appropriate actions based on relevant law and industry codes of ethical behaviour</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Cognitive</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>Understanding</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>[('analyse', 'Analysing'), ('deliberate', 'Verb not mapped'), ('occur', 'Verb not mapped'), ('identify', 'Understanding'), ('base', 'Verb not mapped')]</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>[('model', 'Evaluating'), ('plan', 'Creating'), ('recognise', 'Understanding'), ('identify', 'Understanding'), ('query', 'Analysing')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>apply project evaluation techniques including the triple bottom line against the overall business model and identify the elements of the project life cycle, including planning, controlling, and organizing to allocate resources.</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Cognitive</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>Analysing</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>[('apply', 'Applying'), ('include', 'Verb not mapped'), ('identify', 'Understanding'), ('include', 'Verb not mapped'), ('plan', 'Creating'), ('control', 'Verb not mapped'), ('organize', 'Verb not mapped'), ('allocate', 'Applying')]</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>[('measure', 'Evaluating'), ('optimise', 'Analysing'), ('determine', 'Analysing'), ('apply', 'Applying'), ('analyse', 'Analysing')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="n">
+        <v>82</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>evaluate and apply the basic tools and techniques to plan, organize, and manage a project and identify strategic constraints in managing the scope, time, cost and quality components.</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>SOLO</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>Relational</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>[('evaluate', 'Extended Abstract'), ('apply', 'Relational'), ('plan', 'Extended Abstract'), ('organize', 'Verb not mapped'), ('manage', 'Relational'), ('identify', 'Unistructural'), ('manage', 'Relational')]</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>[('organise', 'Relational'), ('plan', 'Extended Abstract'), ('identify', 'Unistructural'), ('manage', 'Relational'), ('describe', 'Multistructural')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="n">
+        <v>83</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>evaluate the interconnection of quality, heath, safety, risk and contract management and assess the consequent responsibilities relevant to professional engineering practice.</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>SOLO</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>Relational</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>[('evaluate', 'Extended Abstract'), ('assess', 'Extended Abstract')]</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>[('issue', 'Multistructural'), ('explain', 'Relational'), ('apply', 'Relational'), ('write', 'Unistructural'), ('recognise', 'Unistructural')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="n">
+        <v>84</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>understand and evaluate the need for sustainability and the impact of professional engineering work in the solution of civil engineering problems in environmental context.</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Cognitive</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>Analysing</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>[('understand', 'Verb not mapped'), ('evaluate', 'Evaluating')]</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>[('recognise', 'Understanding'), ('analyse', 'Analysing'), ('compare', 'Understanding'), ('research', 'Analysing'), ('construct', 'Creating')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>explain the contract laws and apply ethical principles and commit to professional ethics and responsibilities and the norms of engineering practice.</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>SOLO</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>Relational</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>[('explain', 'Relational'), ('apply', 'Relational'), ('commit', 'Verb not mapped')]</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>[('apply', 'Relational'), ('define', 'Multistructural'), ('discern', 'Multistructural'), ('explain', 'Relational'), ('engage', 'Extended Abstract')]</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="n">
+        <v>86</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>communicate effectively on complex civil engineering activities with the engineering community in both oral and written form.</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Affective</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>Responding</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>[('communicate', 'Responding')]</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>[('demonstrate', 'Valuing'), ('form', 'Valuing'), ('recognise', 'Receiving'), ('relate', 'Organisation'), ('establish', 'Organisation')]</t>
         </is>
       </c>
     </row>

</xml_diff>